<commit_message>
add rules in xlsx
</commit_message>
<xml_diff>
--- a/chalet.xlsx
+++ b/chalet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039B6736-C590-43FB-942D-2D5E62B65408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572C5E65-B9FF-4BDF-A1F7-6D897ADFBE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="12495" windowWidth="28935" windowHeight="19185" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="12495" windowWidth="28935" windowHeight="19185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pool" sheetId="16" r:id="rId1"/>
     <sheet name="Résultats" sheetId="7" r:id="rId2"/>
+    <sheet name="Règlements" sheetId="17" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Pool!$B$11:$AL$30</definedName>
@@ -1853,7 +1854,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2283,6 +2284,150 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2295,224 +2440,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="103" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2625,6 +2557,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>75601</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>36827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{310FEE0A-0C0E-4CBD-99EE-1342065484C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="161925" y="57150"/>
+          <a:ext cx="4790476" cy="10180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2953,8 +2934,8 @@
   </sheetPr>
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2978,256 +2959,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
-      <c r="I1" s="229"/>
-      <c r="J1" s="229"/>
-      <c r="K1" s="229"/>
-      <c r="L1" s="229"/>
-      <c r="M1" s="229"/>
-      <c r="N1" s="229"/>
-      <c r="O1" s="229"/>
-      <c r="P1" s="230"/>
-      <c r="Q1" s="230"/>
-      <c r="R1" s="230"/>
-      <c r="S1" s="230"/>
-      <c r="T1" s="230"/>
-      <c r="U1" s="230"/>
-      <c r="V1" s="230"/>
-      <c r="W1" s="230"/>
-      <c r="X1" s="230"/>
-      <c r="Y1" s="230"/>
-      <c r="Z1" s="230"/>
-      <c r="AA1" s="230"/>
-      <c r="AB1" s="230"/>
-      <c r="AC1" s="230"/>
-      <c r="AD1" s="230"/>
-      <c r="AE1" s="230"/>
-      <c r="AF1" s="230"/>
-      <c r="AG1" s="230"/>
-      <c r="AH1" s="230"/>
-      <c r="AI1" s="230"/>
-      <c r="AJ1" s="230"/>
+      <c r="C1" s="202"/>
+      <c r="D1" s="202"/>
+      <c r="E1" s="202"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="202"/>
+      <c r="M1" s="202"/>
+      <c r="N1" s="202"/>
+      <c r="O1" s="202"/>
+      <c r="P1" s="203"/>
+      <c r="Q1" s="203"/>
+      <c r="R1" s="203"/>
+      <c r="S1" s="203"/>
+      <c r="T1" s="203"/>
+      <c r="U1" s="203"/>
+      <c r="V1" s="203"/>
+      <c r="W1" s="203"/>
+      <c r="X1" s="203"/>
+      <c r="Y1" s="203"/>
+      <c r="Z1" s="203"/>
+      <c r="AA1" s="203"/>
+      <c r="AB1" s="203"/>
+      <c r="AC1" s="203"/>
+      <c r="AD1" s="203"/>
+      <c r="AE1" s="203"/>
+      <c r="AF1" s="203"/>
+      <c r="AG1" s="203"/>
+      <c r="AH1" s="203"/>
+      <c r="AI1" s="203"/>
+      <c r="AJ1" s="203"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
-      <c r="C2" s="231" t="s">
+      <c r="C2" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="231"/>
-      <c r="E2" s="231"/>
-      <c r="F2" s="231"/>
-      <c r="G2" s="231"/>
-      <c r="H2" s="231"/>
-      <c r="I2" s="231"/>
-      <c r="J2" s="231"/>
-      <c r="K2" s="231"/>
-      <c r="L2" s="231"/>
-      <c r="M2" s="231"/>
-      <c r="N2" s="231"/>
-      <c r="O2" s="231"/>
-      <c r="P2" s="231"/>
-      <c r="Q2" s="232" t="s">
+      <c r="D2" s="204"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="204"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="204"/>
+      <c r="I2" s="204"/>
+      <c r="J2" s="204"/>
+      <c r="K2" s="204"/>
+      <c r="L2" s="204"/>
+      <c r="M2" s="204"/>
+      <c r="N2" s="204"/>
+      <c r="O2" s="204"/>
+      <c r="P2" s="204"/>
+      <c r="Q2" s="205" t="s">
         <v>68</v>
       </c>
-      <c r="R2" s="230"/>
-      <c r="S2" s="230"/>
-      <c r="T2" s="230"/>
-      <c r="U2" s="230"/>
-      <c r="V2" s="230"/>
-      <c r="W2" s="230"/>
-      <c r="X2" s="230"/>
-      <c r="Y2" s="230"/>
-      <c r="Z2" s="230"/>
-      <c r="AA2" s="230"/>
-      <c r="AB2" s="230"/>
-      <c r="AC2" s="230"/>
-      <c r="AD2" s="230"/>
-      <c r="AE2" s="230"/>
-      <c r="AF2" s="230"/>
-      <c r="AG2" s="230"/>
-      <c r="AH2" s="230"/>
-      <c r="AI2" s="230"/>
-      <c r="AJ2" s="230"/>
+      <c r="R2" s="203"/>
+      <c r="S2" s="203"/>
+      <c r="T2" s="203"/>
+      <c r="U2" s="203"/>
+      <c r="V2" s="203"/>
+      <c r="W2" s="203"/>
+      <c r="X2" s="203"/>
+      <c r="Y2" s="203"/>
+      <c r="Z2" s="203"/>
+      <c r="AA2" s="203"/>
+      <c r="AB2" s="203"/>
+      <c r="AC2" s="203"/>
+      <c r="AD2" s="203"/>
+      <c r="AE2" s="203"/>
+      <c r="AF2" s="203"/>
+      <c r="AG2" s="203"/>
+      <c r="AH2" s="203"/>
+      <c r="AI2" s="203"/>
+      <c r="AJ2" s="203"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
-      <c r="C3" s="231" t="s">
+      <c r="C3" s="204" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="231"/>
-      <c r="E3" s="231"/>
-      <c r="F3" s="231"/>
-      <c r="G3" s="231"/>
-      <c r="H3" s="231"/>
-      <c r="I3" s="231"/>
-      <c r="J3" s="231"/>
-      <c r="K3" s="231"/>
-      <c r="L3" s="231"/>
-      <c r="M3" s="231"/>
-      <c r="N3" s="231"/>
-      <c r="O3" s="231"/>
-      <c r="P3" s="231"/>
-      <c r="Q3" s="232" t="s">
+      <c r="D3" s="204"/>
+      <c r="E3" s="204"/>
+      <c r="F3" s="204"/>
+      <c r="G3" s="204"/>
+      <c r="H3" s="204"/>
+      <c r="I3" s="204"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
+      <c r="L3" s="204"/>
+      <c r="M3" s="204"/>
+      <c r="N3" s="204"/>
+      <c r="O3" s="204"/>
+      <c r="P3" s="204"/>
+      <c r="Q3" s="205" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="230"/>
-      <c r="S3" s="230"/>
-      <c r="T3" s="230"/>
-      <c r="U3" s="230"/>
-      <c r="V3" s="230"/>
-      <c r="W3" s="230"/>
-      <c r="X3" s="230"/>
-      <c r="Y3" s="230"/>
-      <c r="Z3" s="230"/>
-      <c r="AA3" s="230"/>
-      <c r="AB3" s="230"/>
-      <c r="AC3" s="230"/>
-      <c r="AD3" s="230"/>
-      <c r="AE3" s="230"/>
-      <c r="AF3" s="230"/>
-      <c r="AG3" s="230"/>
-      <c r="AH3" s="230"/>
-      <c r="AI3" s="230"/>
-      <c r="AJ3" s="230"/>
+      <c r="R3" s="203"/>
+      <c r="S3" s="203"/>
+      <c r="T3" s="203"/>
+      <c r="U3" s="203"/>
+      <c r="V3" s="203"/>
+      <c r="W3" s="203"/>
+      <c r="X3" s="203"/>
+      <c r="Y3" s="203"/>
+      <c r="Z3" s="203"/>
+      <c r="AA3" s="203"/>
+      <c r="AB3" s="203"/>
+      <c r="AC3" s="203"/>
+      <c r="AD3" s="203"/>
+      <c r="AE3" s="203"/>
+      <c r="AF3" s="203"/>
+      <c r="AG3" s="203"/>
+      <c r="AH3" s="203"/>
+      <c r="AI3" s="203"/>
+      <c r="AJ3" s="203"/>
     </row>
     <row r="4" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="229"/>
-      <c r="D4" s="229"/>
-      <c r="E4" s="229"/>
-      <c r="F4" s="229"/>
-      <c r="G4" s="229"/>
-      <c r="H4" s="229"/>
-      <c r="I4" s="229"/>
-      <c r="J4" s="229"/>
-      <c r="K4" s="229"/>
-      <c r="L4" s="229"/>
-      <c r="M4" s="229"/>
-      <c r="N4" s="229"/>
-      <c r="O4" s="229"/>
-      <c r="P4" s="230"/>
-      <c r="Q4" s="230"/>
-      <c r="R4" s="230"/>
-      <c r="S4" s="230"/>
-      <c r="T4" s="230"/>
-      <c r="U4" s="230"/>
-      <c r="V4" s="230"/>
-      <c r="W4" s="230"/>
-      <c r="X4" s="230"/>
-      <c r="Y4" s="230"/>
-      <c r="Z4" s="230"/>
-      <c r="AA4" s="230"/>
-      <c r="AB4" s="230"/>
-      <c r="AC4" s="230"/>
-      <c r="AD4" s="230"/>
-      <c r="AE4" s="230"/>
-      <c r="AF4" s="230"/>
-      <c r="AG4" s="230"/>
-      <c r="AH4" s="230"/>
-      <c r="AI4" s="230"/>
-      <c r="AJ4" s="230"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
+      <c r="N4" s="202"/>
+      <c r="O4" s="202"/>
+      <c r="P4" s="203"/>
+      <c r="Q4" s="203"/>
+      <c r="R4" s="203"/>
+      <c r="S4" s="203"/>
+      <c r="T4" s="203"/>
+      <c r="U4" s="203"/>
+      <c r="V4" s="203"/>
+      <c r="W4" s="203"/>
+      <c r="X4" s="203"/>
+      <c r="Y4" s="203"/>
+      <c r="Z4" s="203"/>
+      <c r="AA4" s="203"/>
+      <c r="AB4" s="203"/>
+      <c r="AC4" s="203"/>
+      <c r="AD4" s="203"/>
+      <c r="AE4" s="203"/>
+      <c r="AF4" s="203"/>
+      <c r="AG4" s="203"/>
+      <c r="AH4" s="203"/>
+      <c r="AI4" s="203"/>
+      <c r="AJ4" s="203"/>
     </row>
     <row r="5" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="233" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="234"/>
-      <c r="E5" s="234"/>
-      <c r="F5" s="234"/>
-      <c r="G5" s="234"/>
-      <c r="H5" s="234"/>
-      <c r="I5" s="234"/>
-      <c r="J5" s="234"/>
-      <c r="K5" s="234"/>
-      <c r="L5" s="234"/>
-      <c r="M5" s="234"/>
-      <c r="N5" s="234"/>
-      <c r="O5" s="234"/>
-      <c r="P5" s="234"/>
-      <c r="Q5" s="234"/>
-      <c r="R5" s="234"/>
-      <c r="S5" s="235"/>
-      <c r="T5" s="233" t="s">
+      <c r="C5" s="189" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="190"/>
+      <c r="E5" s="190"/>
+      <c r="F5" s="190"/>
+      <c r="G5" s="190"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="190"/>
+      <c r="K5" s="190"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="N5" s="190"/>
+      <c r="O5" s="190"/>
+      <c r="P5" s="190"/>
+      <c r="Q5" s="190"/>
+      <c r="R5" s="190"/>
+      <c r="S5" s="191"/>
+      <c r="T5" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="234"/>
-      <c r="V5" s="234"/>
-      <c r="W5" s="234"/>
-      <c r="X5" s="234"/>
-      <c r="Y5" s="234"/>
-      <c r="Z5" s="234"/>
-      <c r="AA5" s="234"/>
-      <c r="AB5" s="235"/>
-      <c r="AC5" s="233" t="s">
+      <c r="U5" s="190"/>
+      <c r="V5" s="190"/>
+      <c r="W5" s="190"/>
+      <c r="X5" s="190"/>
+      <c r="Y5" s="190"/>
+      <c r="Z5" s="190"/>
+      <c r="AA5" s="190"/>
+      <c r="AB5" s="191"/>
+      <c r="AC5" s="189" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="234"/>
-      <c r="AE5" s="234"/>
-      <c r="AF5" s="234"/>
-      <c r="AG5" s="236"/>
-      <c r="AH5" s="233" t="s">
+      <c r="AD5" s="190"/>
+      <c r="AE5" s="190"/>
+      <c r="AF5" s="190"/>
+      <c r="AG5" s="192"/>
+      <c r="AH5" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="AI5" s="234"/>
-      <c r="AJ5" s="235"/>
+      <c r="AI5" s="190"/>
+      <c r="AJ5" s="191"/>
     </row>
     <row r="6" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="206" t="s">
+      <c r="C6" s="193" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="201"/>
-      <c r="E6" s="201"/>
-      <c r="F6" s="201"/>
-      <c r="G6" s="201"/>
-      <c r="H6" s="201"/>
-      <c r="I6" s="201"/>
-      <c r="J6" s="202"/>
+      <c r="D6" s="194"/>
+      <c r="E6" s="194"/>
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="194"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="195"/>
       <c r="K6" s="200" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="201"/>
-      <c r="M6" s="201"/>
-      <c r="N6" s="201"/>
-      <c r="O6" s="201"/>
-      <c r="P6" s="201"/>
-      <c r="Q6" s="201"/>
-      <c r="R6" s="202"/>
-      <c r="S6" s="203" t="s">
+      <c r="L6" s="194"/>
+      <c r="M6" s="194"/>
+      <c r="N6" s="194"/>
+      <c r="O6" s="194"/>
+      <c r="P6" s="194"/>
+      <c r="Q6" s="194"/>
+      <c r="R6" s="195"/>
+      <c r="S6" s="196" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="206" t="s">
+      <c r="T6" s="193" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="201"/>
-      <c r="V6" s="201"/>
-      <c r="W6" s="202"/>
+      <c r="U6" s="194"/>
+      <c r="V6" s="194"/>
+      <c r="W6" s="195"/>
       <c r="X6" s="200" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="201"/>
-      <c r="Z6" s="201"/>
-      <c r="AA6" s="202"/>
-      <c r="AB6" s="203" t="s">
+      <c r="Y6" s="194"/>
+      <c r="Z6" s="194"/>
+      <c r="AA6" s="195"/>
+      <c r="AB6" s="196" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="238" t="s">
+      <c r="AC6" s="201" t="s">
         <v>9</v>
       </c>
-      <c r="AD6" s="202"/>
+      <c r="AD6" s="195"/>
       <c r="AE6" s="200" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="202"/>
-      <c r="AG6" s="203" t="s">
+      <c r="AF6" s="195"/>
+      <c r="AG6" s="196" t="s">
         <v>14</v>
       </c>
       <c r="AH6" s="46"/>
       <c r="AI6" s="21"/>
-      <c r="AJ6" s="203" t="s">
+      <c r="AJ6" s="196" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3237,11 +3218,11 @@
         <f>Résultats!$J$3</f>
         <v>2</v>
       </c>
-      <c r="D7" s="239">
+      <c r="D7" s="76">
         <f>Résultats!$J$4</f>
         <v>1</v>
       </c>
-      <c r="E7" s="243">
+      <c r="E7" s="118">
         <f>Résultats!$J$6</f>
         <v>1</v>
       </c>
@@ -3253,11 +3234,11 @@
         <f>Résultats!$J$10</f>
         <v>2</v>
       </c>
-      <c r="H7" s="247">
+      <c r="H7" s="77">
         <f>Résultats!$J$11</f>
         <v>1</v>
       </c>
-      <c r="I7" s="243">
+      <c r="I7" s="118">
         <f>Résultats!$J$13</f>
         <v>0</v>
       </c>
@@ -3269,7 +3250,7 @@
         <f>Résultats!$J$17</f>
         <v>1</v>
       </c>
-      <c r="L7" s="239">
+      <c r="L7" s="76">
         <f>Résultats!$J$18</f>
         <v>1</v>
       </c>
@@ -3277,7 +3258,7 @@
         <f>Résultats!$J$20</f>
         <v>1</v>
       </c>
-      <c r="N7" s="247">
+      <c r="N7" s="77">
         <f>Résultats!$J$21</f>
         <v>2</v>
       </c>
@@ -3285,11 +3266,11 @@
         <f>Résultats!$J$24</f>
         <v>1</v>
       </c>
-      <c r="P7" s="247">
+      <c r="P7" s="77">
         <f>Résultats!$J$25</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="251">
+      <c r="Q7" s="187">
         <f>Résultats!$J$27</f>
         <v>1</v>
       </c>
@@ -3297,8 +3278,8 @@
         <f>Résultats!$J$28</f>
         <v>2</v>
       </c>
-      <c r="S7" s="204"/>
-      <c r="T7" s="255">
+      <c r="S7" s="197"/>
+      <c r="T7" s="115">
         <f>Résultats!$V$6</f>
         <v>0</v>
       </c>
@@ -3310,11 +3291,11 @@
         <f>Résultats!$V$10</f>
         <v>0</v>
       </c>
-      <c r="W7" s="239">
+      <c r="W7" s="76">
         <f>Résultats!$V$11</f>
         <v>0</v>
       </c>
-      <c r="X7" s="259">
+      <c r="X7" s="78">
         <f>Résultats!$V$20</f>
         <v>0</v>
       </c>
@@ -3322,7 +3303,7 @@
         <f>Résultats!$V$21</f>
         <v>0</v>
       </c>
-      <c r="Z7" s="251">
+      <c r="Z7" s="187">
         <f>Résultats!$V$24</f>
         <v>0</v>
       </c>
@@ -3330,8 +3311,8 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB7" s="204"/>
-      <c r="AC7" s="251">
+      <c r="AB7" s="197"/>
+      <c r="AC7" s="187">
         <f>Résultats!$AH$8</f>
         <v>0</v>
       </c>
@@ -3343,11 +3324,11 @@
         <f>Résultats!$AH$22</f>
         <v>0</v>
       </c>
-      <c r="AF7" s="239">
+      <c r="AF7" s="76">
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="204"/>
+      <c r="AG7" s="197"/>
       <c r="AH7" s="132">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -3356,7 +3337,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ7" s="204"/>
+      <c r="AJ7" s="197"/>
     </row>
     <row r="8" spans="1:38" s="31" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32"/>
@@ -3365,39 +3346,39 @@
 +IF(ISBLANK($D11),0,($D$7*PT_VICTOIRE_R1)+IF($D$7=4,PT_PREDICTION_EQUIPE_R1+IF($D11=$C$7+$D$7,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>0</v>
       </c>
-      <c r="D8" s="240"/>
-      <c r="E8" s="244"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="119"/>
       <c r="F8" s="84"/>
       <c r="G8" s="85"/>
-      <c r="H8" s="240"/>
-      <c r="I8" s="244"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="119"/>
       <c r="J8" s="83"/>
       <c r="K8" s="86"/>
-      <c r="L8" s="240"/>
+      <c r="L8" s="83"/>
       <c r="M8" s="119"/>
-      <c r="N8" s="248"/>
+      <c r="N8" s="84"/>
       <c r="O8" s="119"/>
-      <c r="P8" s="248"/>
-      <c r="Q8" s="252"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="85"/>
       <c r="R8" s="83"/>
-      <c r="S8" s="204"/>
-      <c r="T8" s="256"/>
+      <c r="S8" s="197"/>
+      <c r="T8" s="116"/>
       <c r="U8" s="83"/>
       <c r="V8" s="119"/>
-      <c r="W8" s="240"/>
-      <c r="X8" s="260"/>
+      <c r="W8" s="83"/>
+      <c r="X8" s="86"/>
       <c r="Y8" s="84"/>
-      <c r="Z8" s="252"/>
+      <c r="Z8" s="85"/>
       <c r="AA8" s="83"/>
-      <c r="AB8" s="204"/>
-      <c r="AC8" s="252"/>
+      <c r="AB8" s="197"/>
+      <c r="AC8" s="85"/>
       <c r="AD8" s="83"/>
       <c r="AE8" s="86"/>
-      <c r="AF8" s="240"/>
-      <c r="AG8" s="204"/>
+      <c r="AF8" s="83"/>
+      <c r="AG8" s="197"/>
       <c r="AH8" s="132"/>
       <c r="AI8" s="79"/>
-      <c r="AJ8" s="204"/>
+      <c r="AJ8" s="197"/>
     </row>
     <row r="9" spans="1:38" s="31" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
@@ -3405,11 +3386,11 @@
         <f>Résultats!$B$3</f>
         <v>BOSTON</v>
       </c>
-      <c r="D9" s="241" t="str">
+      <c r="D9" s="120" t="str">
         <f>Résultats!$B$4</f>
         <v>FLORIDA</v>
       </c>
-      <c r="E9" s="245" t="str">
+      <c r="E9" s="121" t="str">
         <f>Résultats!$B$6</f>
         <v>TORONTO</v>
       </c>
@@ -3421,11 +3402,11 @@
         <f>Résultats!$B$10</f>
         <v>CAROLINA</v>
       </c>
-      <c r="H9" s="241" t="str">
+      <c r="H9" s="120" t="str">
         <f>Résultats!$B$11</f>
         <v>NY ISLANDERS</v>
       </c>
-      <c r="I9" s="245" t="str">
+      <c r="I9" s="121" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW JERSEY</v>
       </c>
@@ -3437,7 +3418,7 @@
         <f>Résultats!$B$17</f>
         <v>COLORADO</v>
       </c>
-      <c r="L9" s="241" t="str">
+      <c r="L9" s="120" t="str">
         <f>Résultats!$B$18</f>
         <v>SEATTLE</v>
       </c>
@@ -3445,7 +3426,7 @@
         <f>Résultats!$B$20</f>
         <v>DALLAS</v>
       </c>
-      <c r="N9" s="249" t="str">
+      <c r="N9" s="122" t="str">
         <f>Résultats!$B$21</f>
         <v>MINNESOTA</v>
       </c>
@@ -3453,11 +3434,11 @@
         <f>Résultats!$B$24</f>
         <v>VEGAS</v>
       </c>
-      <c r="P9" s="249" t="str">
+      <c r="P9" s="122" t="str">
         <f>Résultats!$B$25</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="Q9" s="253" t="str">
+      <c r="Q9" s="123" t="str">
         <f>Résultats!$B$27</f>
         <v>EDMONTON</v>
       </c>
@@ -3465,8 +3446,8 @@
         <f>Résultats!$B$28</f>
         <v>LOS ANGELES</v>
       </c>
-      <c r="S9" s="204"/>
-      <c r="T9" s="257">
+      <c r="S9" s="197"/>
+      <c r="T9" s="117">
         <f>Résultats!$N$6</f>
         <v>0</v>
       </c>
@@ -3478,11 +3459,11 @@
         <f>Résultats!$N$10</f>
         <v>0</v>
       </c>
-      <c r="W9" s="241">
+      <c r="W9" s="120">
         <f>Résultats!$N$11</f>
         <v>0</v>
       </c>
-      <c r="X9" s="261">
+      <c r="X9" s="124">
         <f>Résultats!$N$20</f>
         <v>0</v>
       </c>
@@ -3490,7 +3471,7 @@
         <f>Résultats!$N$21</f>
         <v>0</v>
       </c>
-      <c r="Z9" s="253">
+      <c r="Z9" s="123">
         <f>Résultats!$N$24</f>
         <v>0</v>
       </c>
@@ -3498,8 +3479,8 @@
         <f>Résultats!$N$25</f>
         <v>0</v>
       </c>
-      <c r="AB9" s="204"/>
-      <c r="AC9" s="253">
+      <c r="AB9" s="197"/>
+      <c r="AC9" s="123">
         <f>Résultats!$Z$8</f>
         <v>0</v>
       </c>
@@ -3511,11 +3492,11 @@
         <f>Résultats!$Z$22</f>
         <v>0</v>
       </c>
-      <c r="AF9" s="241">
+      <c r="AF9" s="120">
         <f>Résultats!$Z$23</f>
         <v>0</v>
       </c>
-      <c r="AG9" s="204"/>
+      <c r="AG9" s="197"/>
       <c r="AH9" s="133">
         <f>Résultats!$Z$15</f>
         <v>0</v>
@@ -3524,7 +3505,7 @@
         <f>Résultats!$Z$16</f>
         <v>0</v>
       </c>
-      <c r="AJ9" s="204"/>
+      <c r="AJ9" s="197"/>
     </row>
     <row r="10" spans="1:38" s="31" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
@@ -3537,11 +3518,11 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D10" s="242" t="str">
+      <c r="D10" s="126" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
-      <c r="E10" s="246" t="str">
+      <c r="E10" s="127" t="str">
         <f>Résultats!$A$6</f>
         <v>A2</v>
       </c>
@@ -3553,11 +3534,11 @@
         <f>Résultats!$A$10</f>
         <v>M1</v>
       </c>
-      <c r="H10" s="242" t="str">
+      <c r="H10" s="126" t="str">
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I10" s="246" t="str">
+      <c r="I10" s="127" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -3569,7 +3550,7 @@
         <f>Résultats!$A$17</f>
         <v>C1</v>
       </c>
-      <c r="L10" s="242" t="str">
+      <c r="L10" s="126" t="str">
         <f>Résultats!$A$18</f>
         <v>WC2</v>
       </c>
@@ -3577,7 +3558,7 @@
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
-      <c r="N10" s="250" t="str">
+      <c r="N10" s="128" t="str">
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
@@ -3585,11 +3566,11 @@
         <f>Résultats!$A$24</f>
         <v>P1</v>
       </c>
-      <c r="P10" s="250" t="str">
+      <c r="P10" s="128" t="str">
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q10" s="254" t="str">
+      <c r="Q10" s="129" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
@@ -3597,8 +3578,8 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S10" s="205"/>
-      <c r="T10" s="258" t="str">
+      <c r="S10" s="199"/>
+      <c r="T10" s="125" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
       </c>
@@ -3610,11 +3591,11 @@
         <f>Résultats!$M$10</f>
         <v>M2</v>
       </c>
-      <c r="W10" s="242" t="str">
+      <c r="W10" s="126" t="str">
         <f>Résultats!$M$11</f>
         <v>WC1</v>
       </c>
-      <c r="X10" s="262" t="str">
+      <c r="X10" s="130" t="str">
         <f>Résultats!$M$20</f>
         <v>P2</v>
       </c>
@@ -3622,7 +3603,7 @@
         <f>Résultats!$M$21</f>
         <v>WC2</v>
       </c>
-      <c r="Z10" s="254" t="str">
+      <c r="Z10" s="129" t="str">
         <f>Résultats!$M$24</f>
         <v>C3</v>
       </c>
@@ -3630,8 +3611,8 @@
         <f>Résultats!$M$25</f>
         <v>WC1</v>
       </c>
-      <c r="AB10" s="237"/>
-      <c r="AC10" s="254" t="str">
+      <c r="AB10" s="198"/>
+      <c r="AC10" s="129" t="str">
         <f>Résultats!$Y$8</f>
         <v>A2</v>
       </c>
@@ -3643,11 +3624,11 @@
         <f>Résultats!$Y$22</f>
         <v>P2</v>
       </c>
-      <c r="AF10" s="242" t="str">
+      <c r="AF10" s="126" t="str">
         <f>Résultats!$Y$23</f>
         <v>C3</v>
       </c>
-      <c r="AG10" s="237"/>
+      <c r="AG10" s="198"/>
       <c r="AH10" s="135" t="str">
         <f>Résultats!$Y$15</f>
         <v>A2</v>
@@ -3656,7 +3637,7 @@
         <f>Résultats!$Y$16</f>
         <v>C3</v>
       </c>
-      <c r="AJ10" s="205"/>
+      <c r="AJ10" s="199"/>
       <c r="AK10" s="81" t="s">
         <v>46</v>
       </c>
@@ -5958,7 +5939,7 @@
         <f>MAX($AL$11:$AL$33) - AL27</f>
         <v>0</v>
       </c>
-      <c r="AL27" s="263">
+      <c r="AL27" s="188">
         <f>$S27+$AB27+$AG27+$AJ27</f>
         <v>0</v>
       </c>
@@ -7050,12 +7031,12 @@
     <row r="36" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
       <c r="N36" s="22"/>
-      <c r="O36" s="220" t="s">
+      <c r="O36" s="226" t="s">
         <v>17</v>
       </c>
-      <c r="P36" s="221"/>
-      <c r="Q36" s="221"/>
-      <c r="R36" s="222"/>
+      <c r="P36" s="227"/>
+      <c r="Q36" s="227"/>
+      <c r="R36" s="228"/>
       <c r="AG36" s="25"/>
       <c r="AH36" s="25"/>
       <c r="AI36" s="25"/>
@@ -7064,21 +7045,21 @@
     </row>
     <row r="37" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
-      <c r="B37" s="210" t="s">
+      <c r="B37" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="211"/>
-      <c r="D37" s="211"/>
-      <c r="E37" s="211"/>
-      <c r="F37" s="211"/>
-      <c r="G37" s="211"/>
-      <c r="H37" s="211"/>
-      <c r="I37" s="211"/>
-      <c r="J37" s="211"/>
-      <c r="K37" s="211"/>
-      <c r="L37" s="211"/>
-      <c r="M37" s="211"/>
-      <c r="N37" s="212"/>
+      <c r="C37" s="217"/>
+      <c r="D37" s="217"/>
+      <c r="E37" s="217"/>
+      <c r="F37" s="217"/>
+      <c r="G37" s="217"/>
+      <c r="H37" s="217"/>
+      <c r="I37" s="217"/>
+      <c r="J37" s="217"/>
+      <c r="K37" s="217"/>
+      <c r="L37" s="217"/>
+      <c r="M37" s="217"/>
+      <c r="N37" s="218"/>
       <c r="O37" s="17">
         <v>1</v>
       </c>
@@ -7091,43 +7072,43 @@
       <c r="R37" s="18">
         <v>4</v>
       </c>
-      <c r="U37" s="223" t="s">
+      <c r="U37" s="229" t="s">
         <v>26</v>
       </c>
-      <c r="V37" s="224"/>
-      <c r="W37" s="224"/>
-      <c r="X37" s="224"/>
-      <c r="Y37" s="224"/>
-      <c r="Z37" s="224"/>
-      <c r="AA37" s="224"/>
-      <c r="AB37" s="224"/>
-      <c r="AC37" s="224"/>
-      <c r="AD37" s="225"/>
-      <c r="AG37" s="226" t="s">
+      <c r="V37" s="230"/>
+      <c r="W37" s="230"/>
+      <c r="X37" s="230"/>
+      <c r="Y37" s="230"/>
+      <c r="Z37" s="230"/>
+      <c r="AA37" s="230"/>
+      <c r="AB37" s="230"/>
+      <c r="AC37" s="230"/>
+      <c r="AD37" s="231"/>
+      <c r="AG37" s="232" t="s">
         <v>24</v>
       </c>
-      <c r="AH37" s="227"/>
-      <c r="AI37" s="227"/>
-      <c r="AJ37" s="227"/>
-      <c r="AK37" s="228"/>
+      <c r="AH37" s="233"/>
+      <c r="AI37" s="233"/>
+      <c r="AJ37" s="233"/>
+      <c r="AK37" s="234"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
-      <c r="B38" s="197" t="s">
+      <c r="B38" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="191"/>
-      <c r="D38" s="191"/>
-      <c r="E38" s="191"/>
-      <c r="F38" s="191"/>
-      <c r="G38" s="191"/>
-      <c r="H38" s="191"/>
-      <c r="I38" s="191"/>
-      <c r="J38" s="191"/>
-      <c r="K38" s="191"/>
-      <c r="L38" s="191"/>
-      <c r="M38" s="191"/>
-      <c r="N38" s="192"/>
+      <c r="C38" s="207"/>
+      <c r="D38" s="207"/>
+      <c r="E38" s="207"/>
+      <c r="F38" s="207"/>
+      <c r="G38" s="207"/>
+      <c r="H38" s="207"/>
+      <c r="I38" s="207"/>
+      <c r="J38" s="207"/>
+      <c r="K38" s="207"/>
+      <c r="L38" s="207"/>
+      <c r="M38" s="207"/>
+      <c r="N38" s="208"/>
       <c r="O38" s="16">
         <v>3</v>
       </c>
@@ -7140,49 +7121,49 @@
       <c r="R38" s="19">
         <v>3</v>
       </c>
-      <c r="U38" s="215" t="s">
+      <c r="U38" s="221" t="s">
         <v>20</v>
       </c>
-      <c r="V38" s="216"/>
-      <c r="W38" s="216"/>
-      <c r="X38" s="216"/>
-      <c r="Y38" s="216"/>
-      <c r="Z38" s="216"/>
-      <c r="AA38" s="216"/>
-      <c r="AB38" s="213">
+      <c r="V38" s="222"/>
+      <c r="W38" s="222"/>
+      <c r="X38" s="222"/>
+      <c r="Y38" s="222"/>
+      <c r="Z38" s="222"/>
+      <c r="AA38" s="222"/>
+      <c r="AB38" s="219">
         <v>5</v>
       </c>
-      <c r="AC38" s="213"/>
-      <c r="AD38" s="214"/>
+      <c r="AC38" s="219"/>
+      <c r="AD38" s="220"/>
       <c r="AE38" s="24"/>
       <c r="AF38" s="24"/>
-      <c r="AG38" s="187" t="s">
+      <c r="AG38" s="235" t="s">
         <v>21</v>
       </c>
-      <c r="AH38" s="188"/>
-      <c r="AI38" s="188"/>
-      <c r="AJ38" s="189"/>
+      <c r="AH38" s="236"/>
+      <c r="AI38" s="236"/>
+      <c r="AJ38" s="237"/>
       <c r="AK38" s="142">
         <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="197" t="s">
+      <c r="B39" s="206" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="191"/>
-      <c r="D39" s="191"/>
-      <c r="E39" s="191"/>
-      <c r="F39" s="191"/>
-      <c r="G39" s="191"/>
-      <c r="H39" s="191"/>
-      <c r="I39" s="191"/>
-      <c r="J39" s="191"/>
-      <c r="K39" s="191"/>
-      <c r="L39" s="191"/>
-      <c r="M39" s="191"/>
-      <c r="N39" s="192"/>
+      <c r="C39" s="207"/>
+      <c r="D39" s="207"/>
+      <c r="E39" s="207"/>
+      <c r="F39" s="207"/>
+      <c r="G39" s="207"/>
+      <c r="H39" s="207"/>
+      <c r="I39" s="207"/>
+      <c r="J39" s="207"/>
+      <c r="K39" s="207"/>
+      <c r="L39" s="207"/>
+      <c r="M39" s="207"/>
+      <c r="N39" s="208"/>
       <c r="O39" s="16">
         <v>2</v>
       </c>
@@ -7195,49 +7176,49 @@
       <c r="R39" s="19">
         <v>2</v>
       </c>
-      <c r="U39" s="193" t="s">
+      <c r="U39" s="211" t="s">
         <v>18</v>
       </c>
-      <c r="V39" s="194"/>
-      <c r="W39" s="194"/>
-      <c r="X39" s="194"/>
-      <c r="Y39" s="194"/>
-      <c r="Z39" s="194"/>
-      <c r="AA39" s="194"/>
-      <c r="AB39" s="195">
+      <c r="V39" s="212"/>
+      <c r="W39" s="212"/>
+      <c r="X39" s="212"/>
+      <c r="Y39" s="212"/>
+      <c r="Z39" s="212"/>
+      <c r="AA39" s="212"/>
+      <c r="AB39" s="239">
         <v>20</v>
       </c>
-      <c r="AC39" s="195"/>
-      <c r="AD39" s="196"/>
+      <c r="AC39" s="239"/>
+      <c r="AD39" s="240"/>
       <c r="AE39" s="24"/>
       <c r="AF39" s="24"/>
-      <c r="AG39" s="190" t="s">
+      <c r="AG39" s="238" t="s">
         <v>22</v>
       </c>
-      <c r="AH39" s="191"/>
-      <c r="AI39" s="191"/>
-      <c r="AJ39" s="192"/>
+      <c r="AH39" s="207"/>
+      <c r="AI39" s="207"/>
+      <c r="AJ39" s="208"/>
       <c r="AK39" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29"/>
-      <c r="B40" s="207" t="s">
+      <c r="B40" s="213" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="208"/>
-      <c r="D40" s="208"/>
-      <c r="E40" s="208"/>
-      <c r="F40" s="208"/>
-      <c r="G40" s="208"/>
-      <c r="H40" s="208"/>
-      <c r="I40" s="208"/>
-      <c r="J40" s="208"/>
-      <c r="K40" s="208"/>
-      <c r="L40" s="208"/>
-      <c r="M40" s="208"/>
-      <c r="N40" s="209"/>
+      <c r="C40" s="214"/>
+      <c r="D40" s="214"/>
+      <c r="E40" s="214"/>
+      <c r="F40" s="214"/>
+      <c r="G40" s="214"/>
+      <c r="H40" s="214"/>
+      <c r="I40" s="214"/>
+      <c r="J40" s="214"/>
+      <c r="K40" s="214"/>
+      <c r="L40" s="214"/>
+      <c r="M40" s="214"/>
+      <c r="N40" s="215"/>
       <c r="O40" s="3">
         <v>0</v>
       </c>
@@ -7250,51 +7231,51 @@
       <c r="R40" s="20">
         <v>0</v>
       </c>
-      <c r="U40" s="217" t="s">
+      <c r="U40" s="223" t="s">
         <v>19</v>
       </c>
-      <c r="V40" s="199"/>
-      <c r="W40" s="199"/>
-      <c r="X40" s="199"/>
-      <c r="Y40" s="199"/>
-      <c r="Z40" s="199"/>
-      <c r="AA40" s="199"/>
-      <c r="AB40" s="218">
+      <c r="V40" s="210"/>
+      <c r="W40" s="210"/>
+      <c r="X40" s="210"/>
+      <c r="Y40" s="210"/>
+      <c r="Z40" s="210"/>
+      <c r="AA40" s="210"/>
+      <c r="AB40" s="224">
         <f>AB38*AB39</f>
         <v>100</v>
       </c>
-      <c r="AC40" s="218"/>
-      <c r="AD40" s="219"/>
+      <c r="AC40" s="224"/>
+      <c r="AD40" s="225"/>
       <c r="AE40" s="24"/>
       <c r="AF40" s="24"/>
-      <c r="AG40" s="190" t="s">
+      <c r="AG40" s="238" t="s">
         <v>25</v>
       </c>
-      <c r="AH40" s="191"/>
-      <c r="AI40" s="191"/>
-      <c r="AJ40" s="192"/>
+      <c r="AH40" s="207"/>
+      <c r="AI40" s="207"/>
+      <c r="AJ40" s="208"/>
       <c r="AK40" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG41" s="193" t="s">
+      <c r="AG41" s="211" t="s">
         <v>23</v>
       </c>
-      <c r="AH41" s="194"/>
-      <c r="AI41" s="194"/>
-      <c r="AJ41" s="194"/>
+      <c r="AH41" s="212"/>
+      <c r="AI41" s="212"/>
+      <c r="AJ41" s="212"/>
       <c r="AK41" s="144">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG42" s="198" t="s">
+      <c r="AG42" s="209" t="s">
         <v>19</v>
       </c>
-      <c r="AH42" s="199"/>
-      <c r="AI42" s="199"/>
-      <c r="AJ42" s="199"/>
+      <c r="AH42" s="210"/>
+      <c r="AI42" s="210"/>
+      <c r="AJ42" s="210"/>
       <c r="AK42" s="143">
         <f>SUM(AK38:AK41)</f>
         <v>100</v>
@@ -7306,25 +7287,11 @@
     <sortCondition ref="B11:B30"/>
   </sortState>
   <mergeCells count="40">
-    <mergeCell ref="C5:S5"/>
-    <mergeCell ref="T5:AB5"/>
-    <mergeCell ref="AC5:AG5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AG6:AG10"/>
-    <mergeCell ref="AJ6:AJ10"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="AB6:AB10"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C4:O4"/>
-    <mergeCell ref="P4:AJ4"/>
-    <mergeCell ref="C3:P3"/>
-    <mergeCell ref="Q3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="AG38:AJ38"/>
+    <mergeCell ref="AG40:AJ40"/>
+    <mergeCell ref="AG39:AJ39"/>
+    <mergeCell ref="U39:AA39"/>
+    <mergeCell ref="AB39:AD39"/>
     <mergeCell ref="B39:N39"/>
     <mergeCell ref="AG42:AJ42"/>
     <mergeCell ref="AG41:AJ41"/>
@@ -7341,11 +7308,25 @@
     <mergeCell ref="O36:R36"/>
     <mergeCell ref="U37:AD37"/>
     <mergeCell ref="AG37:AK37"/>
-    <mergeCell ref="AG38:AJ38"/>
-    <mergeCell ref="AG40:AJ40"/>
-    <mergeCell ref="AG39:AJ39"/>
-    <mergeCell ref="U39:AA39"/>
-    <mergeCell ref="AB39:AD39"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C4:O4"/>
+    <mergeCell ref="P4:AJ4"/>
+    <mergeCell ref="C3:P3"/>
+    <mergeCell ref="Q3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
+    <mergeCell ref="C5:S5"/>
+    <mergeCell ref="T5:AB5"/>
+    <mergeCell ref="AC5:AG5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AG6:AG10"/>
+    <mergeCell ref="AJ6:AJ10"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="AB6:AB10"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="C34:D34">
@@ -7554,11 +7535,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL11:AL33">
-    <cfRule type="cellIs" dxfId="8" priority="32" operator="notEqual">
-      <formula>""""""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AK11:AK30">
     <cfRule type="dataBar" priority="46">
       <dataBar>
@@ -7571,6 +7547,11 @@
           <x14:id>{C7C89828-A80F-4CFB-A8E3-6391A56E8618}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL11:AL33">
+    <cfRule type="cellIs" dxfId="8" priority="32" operator="notEqual">
+      <formula>""""""</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -7762,8 +7743,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y48" sqref="Y48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9036,4 +9017,19 @@
 Dernière mise à jour: &amp;D - &amp;T</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2183EB04-0219-41DB-960E-AB532E8842E9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update end of round 1
</commit_message>
<xml_diff>
--- a/chalet.xlsx
+++ b/chalet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9407577C-7422-4A24-85E7-DB3935DAF1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F584C17-C3B2-4128-A689-38EB3CCFCDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="12600" windowWidth="28935" windowHeight="19185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="12495" windowWidth="28935" windowHeight="19185" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pool" sheetId="16" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>RONDE 1</t>
   </si>
@@ -270,7 +270,7 @@
     <numFmt numFmtId="167" formatCode="_ * #,##0_)\ &quot;$&quot;_ ;_ * \(#,##0\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
     <numFmt numFmtId="168" formatCode="_ * #,##0_)\ _$_ ;_ * \(#,##0\)\ _$_ ;_ * &quot;-&quot;??_)\ _$_ ;_ @_ "/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -383,6 +383,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -429,7 +442,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1860,7 +1873,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2275,9 +2288,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2296,6 +2306,45 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2452,49 +2501,22 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2985,8 +3007,8 @@
   </sheetPr>
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X50" sqref="X50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3010,256 +3032,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
-      <c r="H1" s="202"/>
-      <c r="I1" s="202"/>
-      <c r="J1" s="202"/>
-      <c r="K1" s="202"/>
-      <c r="L1" s="202"/>
-      <c r="M1" s="202"/>
-      <c r="N1" s="202"/>
-      <c r="O1" s="202"/>
-      <c r="P1" s="203"/>
-      <c r="Q1" s="203"/>
-      <c r="R1" s="203"/>
-      <c r="S1" s="203"/>
-      <c r="T1" s="203"/>
-      <c r="U1" s="203"/>
-      <c r="V1" s="203"/>
-      <c r="W1" s="203"/>
-      <c r="X1" s="203"/>
-      <c r="Y1" s="203"/>
-      <c r="Z1" s="203"/>
-      <c r="AA1" s="203"/>
-      <c r="AB1" s="203"/>
-      <c r="AC1" s="203"/>
-      <c r="AD1" s="203"/>
-      <c r="AE1" s="203"/>
-      <c r="AF1" s="203"/>
-      <c r="AG1" s="203"/>
-      <c r="AH1" s="203"/>
-      <c r="AI1" s="203"/>
-      <c r="AJ1" s="203"/>
+      <c r="C1" s="214"/>
+      <c r="D1" s="214"/>
+      <c r="E1" s="214"/>
+      <c r="F1" s="214"/>
+      <c r="G1" s="214"/>
+      <c r="H1" s="214"/>
+      <c r="I1" s="214"/>
+      <c r="J1" s="214"/>
+      <c r="K1" s="214"/>
+      <c r="L1" s="214"/>
+      <c r="M1" s="214"/>
+      <c r="N1" s="214"/>
+      <c r="O1" s="214"/>
+      <c r="P1" s="215"/>
+      <c r="Q1" s="215"/>
+      <c r="R1" s="215"/>
+      <c r="S1" s="215"/>
+      <c r="T1" s="215"/>
+      <c r="U1" s="215"/>
+      <c r="V1" s="215"/>
+      <c r="W1" s="215"/>
+      <c r="X1" s="215"/>
+      <c r="Y1" s="215"/>
+      <c r="Z1" s="215"/>
+      <c r="AA1" s="215"/>
+      <c r="AB1" s="215"/>
+      <c r="AC1" s="215"/>
+      <c r="AD1" s="215"/>
+      <c r="AE1" s="215"/>
+      <c r="AF1" s="215"/>
+      <c r="AG1" s="215"/>
+      <c r="AH1" s="215"/>
+      <c r="AI1" s="215"/>
+      <c r="AJ1" s="215"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
-      <c r="C2" s="204" t="s">
+      <c r="C2" s="216" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
-      <c r="I2" s="204"/>
-      <c r="J2" s="204"/>
-      <c r="K2" s="204"/>
-      <c r="L2" s="204"/>
-      <c r="M2" s="204"/>
-      <c r="N2" s="204"/>
-      <c r="O2" s="204"/>
-      <c r="P2" s="204"/>
-      <c r="Q2" s="205" t="s">
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="216"/>
+      <c r="H2" s="216"/>
+      <c r="I2" s="216"/>
+      <c r="J2" s="216"/>
+      <c r="K2" s="216"/>
+      <c r="L2" s="216"/>
+      <c r="M2" s="216"/>
+      <c r="N2" s="216"/>
+      <c r="O2" s="216"/>
+      <c r="P2" s="216"/>
+      <c r="Q2" s="217" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="203"/>
-      <c r="S2" s="203"/>
-      <c r="T2" s="203"/>
-      <c r="U2" s="203"/>
-      <c r="V2" s="203"/>
-      <c r="W2" s="203"/>
-      <c r="X2" s="203"/>
-      <c r="Y2" s="203"/>
-      <c r="Z2" s="203"/>
-      <c r="AA2" s="203"/>
-      <c r="AB2" s="203"/>
-      <c r="AC2" s="203"/>
-      <c r="AD2" s="203"/>
-      <c r="AE2" s="203"/>
-      <c r="AF2" s="203"/>
-      <c r="AG2" s="203"/>
-      <c r="AH2" s="203"/>
-      <c r="AI2" s="203"/>
-      <c r="AJ2" s="203"/>
+      <c r="R2" s="215"/>
+      <c r="S2" s="215"/>
+      <c r="T2" s="215"/>
+      <c r="U2" s="215"/>
+      <c r="V2" s="215"/>
+      <c r="W2" s="215"/>
+      <c r="X2" s="215"/>
+      <c r="Y2" s="215"/>
+      <c r="Z2" s="215"/>
+      <c r="AA2" s="215"/>
+      <c r="AB2" s="215"/>
+      <c r="AC2" s="215"/>
+      <c r="AD2" s="215"/>
+      <c r="AE2" s="215"/>
+      <c r="AF2" s="215"/>
+      <c r="AG2" s="215"/>
+      <c r="AH2" s="215"/>
+      <c r="AI2" s="215"/>
+      <c r="AJ2" s="215"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
-      <c r="C3" s="204" t="s">
+      <c r="C3" s="216" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="204"/>
-      <c r="E3" s="204"/>
-      <c r="F3" s="204"/>
-      <c r="G3" s="204"/>
-      <c r="H3" s="204"/>
-      <c r="I3" s="204"/>
-      <c r="J3" s="204"/>
-      <c r="K3" s="204"/>
-      <c r="L3" s="204"/>
-      <c r="M3" s="204"/>
-      <c r="N3" s="204"/>
-      <c r="O3" s="204"/>
-      <c r="P3" s="204"/>
-      <c r="Q3" s="205" t="s">
+      <c r="D3" s="216"/>
+      <c r="E3" s="216"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
+      <c r="H3" s="216"/>
+      <c r="I3" s="216"/>
+      <c r="J3" s="216"/>
+      <c r="K3" s="216"/>
+      <c r="L3" s="216"/>
+      <c r="M3" s="216"/>
+      <c r="N3" s="216"/>
+      <c r="O3" s="216"/>
+      <c r="P3" s="216"/>
+      <c r="Q3" s="217" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="203"/>
-      <c r="S3" s="203"/>
-      <c r="T3" s="203"/>
-      <c r="U3" s="203"/>
-      <c r="V3" s="203"/>
-      <c r="W3" s="203"/>
-      <c r="X3" s="203"/>
-      <c r="Y3" s="203"/>
-      <c r="Z3" s="203"/>
-      <c r="AA3" s="203"/>
-      <c r="AB3" s="203"/>
-      <c r="AC3" s="203"/>
-      <c r="AD3" s="203"/>
-      <c r="AE3" s="203"/>
-      <c r="AF3" s="203"/>
-      <c r="AG3" s="203"/>
-      <c r="AH3" s="203"/>
-      <c r="AI3" s="203"/>
-      <c r="AJ3" s="203"/>
+      <c r="R3" s="215"/>
+      <c r="S3" s="215"/>
+      <c r="T3" s="215"/>
+      <c r="U3" s="215"/>
+      <c r="V3" s="215"/>
+      <c r="W3" s="215"/>
+      <c r="X3" s="215"/>
+      <c r="Y3" s="215"/>
+      <c r="Z3" s="215"/>
+      <c r="AA3" s="215"/>
+      <c r="AB3" s="215"/>
+      <c r="AC3" s="215"/>
+      <c r="AD3" s="215"/>
+      <c r="AE3" s="215"/>
+      <c r="AF3" s="215"/>
+      <c r="AG3" s="215"/>
+      <c r="AH3" s="215"/>
+      <c r="AI3" s="215"/>
+      <c r="AJ3" s="215"/>
     </row>
     <row r="4" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="202"/>
-      <c r="D4" s="202"/>
-      <c r="E4" s="202"/>
-      <c r="F4" s="202"/>
-      <c r="G4" s="202"/>
-      <c r="H4" s="202"/>
-      <c r="I4" s="202"/>
-      <c r="J4" s="202"/>
-      <c r="K4" s="202"/>
-      <c r="L4" s="202"/>
-      <c r="M4" s="202"/>
-      <c r="N4" s="202"/>
-      <c r="O4" s="202"/>
-      <c r="P4" s="203"/>
-      <c r="Q4" s="203"/>
-      <c r="R4" s="203"/>
-      <c r="S4" s="203"/>
-      <c r="T4" s="203"/>
-      <c r="U4" s="203"/>
-      <c r="V4" s="203"/>
-      <c r="W4" s="203"/>
-      <c r="X4" s="203"/>
-      <c r="Y4" s="203"/>
-      <c r="Z4" s="203"/>
-      <c r="AA4" s="203"/>
-      <c r="AB4" s="203"/>
-      <c r="AC4" s="203"/>
-      <c r="AD4" s="203"/>
-      <c r="AE4" s="203"/>
-      <c r="AF4" s="203"/>
-      <c r="AG4" s="203"/>
-      <c r="AH4" s="203"/>
-      <c r="AI4" s="203"/>
-      <c r="AJ4" s="203"/>
+      <c r="C4" s="214"/>
+      <c r="D4" s="214"/>
+      <c r="E4" s="214"/>
+      <c r="F4" s="214"/>
+      <c r="G4" s="214"/>
+      <c r="H4" s="214"/>
+      <c r="I4" s="214"/>
+      <c r="J4" s="214"/>
+      <c r="K4" s="214"/>
+      <c r="L4" s="214"/>
+      <c r="M4" s="214"/>
+      <c r="N4" s="214"/>
+      <c r="O4" s="214"/>
+      <c r="P4" s="215"/>
+      <c r="Q4" s="215"/>
+      <c r="R4" s="215"/>
+      <c r="S4" s="215"/>
+      <c r="T4" s="215"/>
+      <c r="U4" s="215"/>
+      <c r="V4" s="215"/>
+      <c r="W4" s="215"/>
+      <c r="X4" s="215"/>
+      <c r="Y4" s="215"/>
+      <c r="Z4" s="215"/>
+      <c r="AA4" s="215"/>
+      <c r="AB4" s="215"/>
+      <c r="AC4" s="215"/>
+      <c r="AD4" s="215"/>
+      <c r="AE4" s="215"/>
+      <c r="AF4" s="215"/>
+      <c r="AG4" s="215"/>
+      <c r="AH4" s="215"/>
+      <c r="AI4" s="215"/>
+      <c r="AJ4" s="215"/>
     </row>
     <row r="5" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="189" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="190"/>
-      <c r="E5" s="190"/>
-      <c r="F5" s="190"/>
-      <c r="G5" s="190"/>
-      <c r="H5" s="190"/>
-      <c r="I5" s="190"/>
-      <c r="J5" s="190"/>
-      <c r="K5" s="190"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
-      <c r="N5" s="190"/>
-      <c r="O5" s="190"/>
-      <c r="P5" s="190"/>
-      <c r="Q5" s="190"/>
-      <c r="R5" s="190"/>
-      <c r="S5" s="191"/>
-      <c r="T5" s="189" t="s">
+      <c r="C5" s="201" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="202"/>
+      <c r="E5" s="202"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="202"/>
+      <c r="J5" s="202"/>
+      <c r="K5" s="202"/>
+      <c r="L5" s="202"/>
+      <c r="M5" s="202"/>
+      <c r="N5" s="202"/>
+      <c r="O5" s="202"/>
+      <c r="P5" s="202"/>
+      <c r="Q5" s="202"/>
+      <c r="R5" s="202"/>
+      <c r="S5" s="203"/>
+      <c r="T5" s="201" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="190"/>
-      <c r="V5" s="190"/>
-      <c r="W5" s="190"/>
-      <c r="X5" s="190"/>
-      <c r="Y5" s="190"/>
-      <c r="Z5" s="190"/>
-      <c r="AA5" s="190"/>
-      <c r="AB5" s="191"/>
-      <c r="AC5" s="189" t="s">
+      <c r="U5" s="202"/>
+      <c r="V5" s="202"/>
+      <c r="W5" s="202"/>
+      <c r="X5" s="202"/>
+      <c r="Y5" s="202"/>
+      <c r="Z5" s="202"/>
+      <c r="AA5" s="202"/>
+      <c r="AB5" s="203"/>
+      <c r="AC5" s="201" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="190"/>
-      <c r="AE5" s="190"/>
-      <c r="AF5" s="190"/>
-      <c r="AG5" s="192"/>
-      <c r="AH5" s="189" t="s">
+      <c r="AD5" s="202"/>
+      <c r="AE5" s="202"/>
+      <c r="AF5" s="202"/>
+      <c r="AG5" s="204"/>
+      <c r="AH5" s="201" t="s">
         <v>10</v>
       </c>
-      <c r="AI5" s="190"/>
-      <c r="AJ5" s="191"/>
+      <c r="AI5" s="202"/>
+      <c r="AJ5" s="203"/>
     </row>
     <row r="6" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="193" t="s">
+      <c r="C6" s="205" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="194"/>
-      <c r="E6" s="194"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="194"/>
-      <c r="H6" s="194"/>
-      <c r="I6" s="194"/>
-      <c r="J6" s="195"/>
-      <c r="K6" s="200" t="s">
+      <c r="D6" s="206"/>
+      <c r="E6" s="206"/>
+      <c r="F6" s="206"/>
+      <c r="G6" s="206"/>
+      <c r="H6" s="206"/>
+      <c r="I6" s="206"/>
+      <c r="J6" s="207"/>
+      <c r="K6" s="212" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="194"/>
-      <c r="M6" s="194"/>
-      <c r="N6" s="194"/>
-      <c r="O6" s="194"/>
-      <c r="P6" s="194"/>
-      <c r="Q6" s="194"/>
-      <c r="R6" s="195"/>
-      <c r="S6" s="196" t="s">
+      <c r="L6" s="206"/>
+      <c r="M6" s="206"/>
+      <c r="N6" s="206"/>
+      <c r="O6" s="206"/>
+      <c r="P6" s="206"/>
+      <c r="Q6" s="206"/>
+      <c r="R6" s="207"/>
+      <c r="S6" s="208" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="193" t="s">
+      <c r="T6" s="205" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="194"/>
-      <c r="V6" s="194"/>
-      <c r="W6" s="195"/>
-      <c r="X6" s="200" t="s">
+      <c r="U6" s="206"/>
+      <c r="V6" s="206"/>
+      <c r="W6" s="207"/>
+      <c r="X6" s="212" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="194"/>
-      <c r="Z6" s="194"/>
-      <c r="AA6" s="195"/>
-      <c r="AB6" s="196" t="s">
+      <c r="Y6" s="206"/>
+      <c r="Z6" s="206"/>
+      <c r="AA6" s="207"/>
+      <c r="AB6" s="208" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="201" t="s">
+      <c r="AC6" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="AD6" s="195"/>
-      <c r="AE6" s="200" t="s">
+      <c r="AD6" s="207"/>
+      <c r="AE6" s="212" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="195"/>
-      <c r="AG6" s="196" t="s">
+      <c r="AF6" s="207"/>
+      <c r="AG6" s="208" t="s">
         <v>14</v>
       </c>
       <c r="AH6" s="46"/>
       <c r="AI6" s="21"/>
-      <c r="AJ6" s="196" t="s">
+      <c r="AJ6" s="208" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3269,11 +3291,11 @@
         <f>Résultats!$J$3</f>
         <v>3</v>
       </c>
-      <c r="D7" s="241">
+      <c r="D7" s="189">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
-      <c r="E7" s="245">
+      <c r="E7" s="193">
         <f>Résultats!$J$6</f>
         <v>4</v>
       </c>
@@ -3281,7 +3303,7 @@
         <f>Résultats!$J$7</f>
         <v>2</v>
       </c>
-      <c r="G7" s="245">
+      <c r="G7" s="193">
         <f>Résultats!$J$10</f>
         <v>4</v>
       </c>
@@ -3289,9 +3311,9 @@
         <f>Résultats!$J$11</f>
         <v>2</v>
       </c>
-      <c r="I7" s="118">
+      <c r="I7" s="193">
         <f>Résultats!$J$13</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7" s="76">
         <f>Résultats!$J$14</f>
@@ -3301,11 +3323,11 @@
         <f>Résultats!$J$17</f>
         <v>3</v>
       </c>
-      <c r="L7" s="241">
+      <c r="L7" s="189">
         <f>Résultats!$J$18</f>
         <v>4</v>
       </c>
-      <c r="M7" s="245">
+      <c r="M7" s="193">
         <f>Résultats!$J$20</f>
         <v>4</v>
       </c>
@@ -3313,7 +3335,7 @@
         <f>Résultats!$J$21</f>
         <v>2</v>
       </c>
-      <c r="O7" s="245">
+      <c r="O7" s="193">
         <f>Résultats!$J$24</f>
         <v>4</v>
       </c>
@@ -3321,7 +3343,7 @@
         <f>Résultats!$J$25</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="252">
+      <c r="Q7" s="200">
         <f>Résultats!$J$27</f>
         <v>4</v>
       </c>
@@ -3329,7 +3351,7 @@
         <f>Résultats!$J$28</f>
         <v>2</v>
       </c>
-      <c r="S7" s="197"/>
+      <c r="S7" s="209"/>
       <c r="T7" s="115">
         <f>Résultats!$V$6</f>
         <v>0</v>
@@ -3354,7 +3376,7 @@
         <f>Résultats!$V$21</f>
         <v>0</v>
       </c>
-      <c r="Z7" s="187">
+      <c r="Z7" s="186">
         <f>Résultats!$V$24</f>
         <v>0</v>
       </c>
@@ -3362,8 +3384,8 @@
         <f>Résultats!$V$25</f>
         <v>0</v>
       </c>
-      <c r="AB7" s="197"/>
-      <c r="AC7" s="187">
+      <c r="AB7" s="209"/>
+      <c r="AC7" s="186">
         <f>Résultats!$AH$8</f>
         <v>0</v>
       </c>
@@ -3379,7 +3401,7 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="197"/>
+      <c r="AG7" s="209"/>
       <c r="AH7" s="132">
         <f>Résultats!$AH$15</f>
         <v>0</v>
@@ -3388,7 +3410,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ7" s="197"/>
+      <c r="AJ7" s="209"/>
     </row>
     <row r="8" spans="1:38" s="31" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32"/>
@@ -3397,22 +3419,22 @@
 +IF(ISBLANK($D11),0,($D$7*PT_VICTOIRE_R1)+IF($D$7=4,PT_PREDICTION_EQUIPE_R1+IF($D11=$C$7+$D$7,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>5</v>
       </c>
-      <c r="D8" s="242"/>
-      <c r="E8" s="246"/>
+      <c r="D8" s="190"/>
+      <c r="E8" s="194"/>
       <c r="F8" s="84"/>
-      <c r="G8" s="249"/>
+      <c r="G8" s="197"/>
       <c r="H8" s="83"/>
-      <c r="I8" s="119"/>
+      <c r="I8" s="194"/>
       <c r="J8" s="83"/>
       <c r="K8" s="86"/>
-      <c r="L8" s="242"/>
-      <c r="M8" s="246"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="194"/>
       <c r="N8" s="84"/>
-      <c r="O8" s="246"/>
+      <c r="O8" s="194"/>
       <c r="P8" s="84"/>
-      <c r="Q8" s="249"/>
+      <c r="Q8" s="197"/>
       <c r="R8" s="83"/>
-      <c r="S8" s="197"/>
+      <c r="S8" s="209"/>
       <c r="T8" s="116"/>
       <c r="U8" s="83"/>
       <c r="V8" s="119"/>
@@ -3421,15 +3443,15 @@
       <c r="Y8" s="84"/>
       <c r="Z8" s="85"/>
       <c r="AA8" s="83"/>
-      <c r="AB8" s="197"/>
+      <c r="AB8" s="209"/>
       <c r="AC8" s="85"/>
       <c r="AD8" s="83"/>
       <c r="AE8" s="86"/>
       <c r="AF8" s="83"/>
-      <c r="AG8" s="197"/>
+      <c r="AG8" s="209"/>
       <c r="AH8" s="132"/>
       <c r="AI8" s="79"/>
-      <c r="AJ8" s="197"/>
+      <c r="AJ8" s="209"/>
     </row>
     <row r="9" spans="1:38" s="31" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
@@ -3437,11 +3459,11 @@
         <f>Résultats!$B$3</f>
         <v>BOSTON</v>
       </c>
-      <c r="D9" s="243" t="str">
+      <c r="D9" s="191" t="str">
         <f>Résultats!$B$4</f>
         <v>FLORIDA</v>
       </c>
-      <c r="E9" s="247" t="str">
+      <c r="E9" s="195" t="str">
         <f>Résultats!$B$6</f>
         <v>TORONTO</v>
       </c>
@@ -3449,7 +3471,7 @@
         <f>Résultats!$B$7</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="G9" s="250" t="str">
+      <c r="G9" s="198" t="str">
         <f>Résultats!$B$10</f>
         <v>CAROLINA</v>
       </c>
@@ -3457,7 +3479,7 @@
         <f>Résultats!$B$11</f>
         <v>NY ISLANDERS</v>
       </c>
-      <c r="I9" s="121" t="str">
+      <c r="I9" s="195" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW JERSEY</v>
       </c>
@@ -3469,11 +3491,11 @@
         <f>Résultats!$B$17</f>
         <v>COLORADO</v>
       </c>
-      <c r="L9" s="243" t="str">
+      <c r="L9" s="191" t="str">
         <f>Résultats!$B$18</f>
         <v>SEATTLE</v>
       </c>
-      <c r="M9" s="247" t="str">
+      <c r="M9" s="195" t="str">
         <f>Résultats!$B$20</f>
         <v>DALLAS</v>
       </c>
@@ -3481,7 +3503,7 @@
         <f>Résultats!$B$21</f>
         <v>MINNESOTA</v>
       </c>
-      <c r="O9" s="247" t="str">
+      <c r="O9" s="195" t="str">
         <f>Résultats!$B$24</f>
         <v>VEGAS</v>
       </c>
@@ -3489,7 +3511,7 @@
         <f>Résultats!$B$25</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="Q9" s="250" t="str">
+      <c r="Q9" s="198" t="str">
         <f>Résultats!$B$27</f>
         <v>EDMONTON</v>
       </c>
@@ -3497,40 +3519,40 @@
         <f>Résultats!$B$28</f>
         <v>LOS ANGELES</v>
       </c>
-      <c r="S9" s="197"/>
-      <c r="T9" s="117">
+      <c r="S9" s="209"/>
+      <c r="T9" s="117" t="str">
         <f>Résultats!$N$6</f>
-        <v>0</v>
-      </c>
-      <c r="U9" s="120">
+        <v>TORONTO</v>
+      </c>
+      <c r="U9" s="120" t="str">
         <f>Résultats!$N$7</f>
-        <v>0</v>
-      </c>
-      <c r="V9" s="121">
+        <v>FLORIDA</v>
+      </c>
+      <c r="V9" s="121" t="str">
         <f>Résultats!$N$10</f>
-        <v>0</v>
-      </c>
-      <c r="W9" s="120">
+        <v>CAROLINA</v>
+      </c>
+      <c r="W9" s="120" t="str">
         <f>Résultats!$N$11</f>
-        <v>0</v>
-      </c>
-      <c r="X9" s="124">
+        <v>NEW JERSEY</v>
+      </c>
+      <c r="X9" s="124" t="str">
         <f>Résultats!$N$20</f>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="122">
+        <v>DALLAS</v>
+      </c>
+      <c r="Y9" s="122" t="str">
         <f>Résultats!$N$21</f>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="123">
+        <v>SEATTLE</v>
+      </c>
+      <c r="Z9" s="123" t="str">
         <f>Résultats!$N$24</f>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="120">
+        <v>VEGAS</v>
+      </c>
+      <c r="AA9" s="120" t="str">
         <f>Résultats!$N$25</f>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="197"/>
+        <v>EDMONTON</v>
+      </c>
+      <c r="AB9" s="209"/>
       <c r="AC9" s="123">
         <f>Résultats!$Z$8</f>
         <v>0</v>
@@ -3547,7 +3569,7 @@
         <f>Résultats!$Z$23</f>
         <v>0</v>
       </c>
-      <c r="AG9" s="197"/>
+      <c r="AG9" s="209"/>
       <c r="AH9" s="133">
         <f>Résultats!$Z$15</f>
         <v>0</v>
@@ -3556,7 +3578,7 @@
         <f>Résultats!$Z$16</f>
         <v>0</v>
       </c>
-      <c r="AJ9" s="197"/>
+      <c r="AJ9" s="209"/>
     </row>
     <row r="10" spans="1:38" s="31" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
@@ -3569,11 +3591,11 @@
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D10" s="244" t="str">
+      <c r="D10" s="192" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
-      <c r="E10" s="248" t="str">
+      <c r="E10" s="196" t="str">
         <f>Résultats!$A$6</f>
         <v>A2</v>
       </c>
@@ -3581,7 +3603,7 @@
         <f>Résultats!$A$7</f>
         <v>A3</v>
       </c>
-      <c r="G10" s="251" t="str">
+      <c r="G10" s="199" t="str">
         <f>Résultats!$A$10</f>
         <v>M1</v>
       </c>
@@ -3589,7 +3611,7 @@
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I10" s="127" t="str">
+      <c r="I10" s="196" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
@@ -3601,11 +3623,11 @@
         <f>Résultats!$A$17</f>
         <v>C1</v>
       </c>
-      <c r="L10" s="244" t="str">
+      <c r="L10" s="192" t="str">
         <f>Résultats!$A$18</f>
         <v>WC2</v>
       </c>
-      <c r="M10" s="248" t="str">
+      <c r="M10" s="196" t="str">
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
@@ -3613,7 +3635,7 @@
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
-      <c r="O10" s="248" t="str">
+      <c r="O10" s="196" t="str">
         <f>Résultats!$A$24</f>
         <v>P1</v>
       </c>
@@ -3621,7 +3643,7 @@
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q10" s="251" t="str">
+      <c r="Q10" s="199" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
@@ -3629,7 +3651,7 @@
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S10" s="199"/>
+      <c r="S10" s="211"/>
       <c r="T10" s="125" t="str">
         <f>Résultats!$M$6</f>
         <v>A2</v>
@@ -3640,15 +3662,15 @@
       </c>
       <c r="V10" s="127" t="str">
         <f>Résultats!$M$10</f>
-        <v>M2</v>
+        <v>M1</v>
       </c>
       <c r="W10" s="126" t="str">
         <f>Résultats!$M$11</f>
-        <v>WC1</v>
+        <v>M2</v>
       </c>
       <c r="X10" s="130" t="str">
         <f>Résultats!$M$20</f>
-        <v>P2</v>
+        <v>C2</v>
       </c>
       <c r="Y10" s="128" t="str">
         <f>Résultats!$M$21</f>
@@ -3656,13 +3678,13 @@
       </c>
       <c r="Z10" s="129" t="str">
         <f>Résultats!$M$24</f>
-        <v>C3</v>
+        <v>P1</v>
       </c>
       <c r="AA10" s="131" t="str">
         <f>Résultats!$M$25</f>
-        <v>WC1</v>
-      </c>
-      <c r="AB10" s="198"/>
+        <v>P2</v>
+      </c>
+      <c r="AB10" s="210"/>
       <c r="AC10" s="129" t="str">
         <f>Résultats!$Y$8</f>
         <v>A2</v>
@@ -3679,7 +3701,7 @@
         <f>Résultats!$Y$23</f>
         <v>C3</v>
       </c>
-      <c r="AG10" s="198"/>
+      <c r="AG10" s="210"/>
       <c r="AH10" s="135" t="str">
         <f>Résultats!$Y$15</f>
         <v>A2</v>
@@ -3688,7 +3710,7 @@
         <f>Résultats!$Y$16</f>
         <v>C3</v>
       </c>
-      <c r="AJ10" s="199"/>
+      <c r="AJ10" s="211"/>
       <c r="AK10" s="81" t="s">
         <v>46</v>
       </c>
@@ -3705,10 +3727,10 @@
         <v>67</v>
       </c>
       <c r="C11" s="150"/>
-      <c r="D11" s="183">
+      <c r="D11" s="254">
         <v>7</v>
       </c>
-      <c r="E11" s="182">
+      <c r="E11" s="255">
         <v>6</v>
       </c>
       <c r="F11" s="151"/>
@@ -3727,12 +3749,12 @@
       <c r="M11" s="152">
         <v>7</v>
       </c>
-      <c r="N11" s="183"/>
-      <c r="O11" s="182">
+      <c r="N11" s="182"/>
+      <c r="O11" s="255">
         <v>5</v>
       </c>
       <c r="P11" s="151"/>
-      <c r="Q11" s="255">
+      <c r="Q11" s="258">
         <v>6</v>
       </c>
       <c r="R11" s="156"/>
@@ -3740,7 +3762,7 @@
         <f>SUM(C12:R12)</f>
         <v>26</v>
       </c>
-      <c r="T11" s="184"/>
+      <c r="T11" s="183"/>
       <c r="U11" s="154"/>
       <c r="V11" s="152"/>
       <c r="W11" s="154"/>
@@ -3760,8 +3782,8 @@
         <f>SUM(AC12:AF12)</f>
         <v>0</v>
       </c>
-      <c r="AH11" s="185"/>
-      <c r="AI11" s="186"/>
+      <c r="AH11" s="184"/>
+      <c r="AI11" s="185"/>
       <c r="AJ11" s="157">
         <f>AH12</f>
         <v>0</v>
@@ -3786,7 +3808,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="96"/>
-      <c r="E12" s="94">
+      <c r="E12" s="256">
         <f>(IF($E11&lt;&gt;"",($E$7*$O$40)+IF($E$7=4,($O$38)+IF($E11=$E$7+$F$7,$O$39,0),0),0)+IF($F11&lt;&gt;"",($F$7*$O$40)+IF($F$7=4,($O$38)+IF($F11=$E$7+$F$7,$O$39,0),0),0))</f>
         <v>5</v>
       </c>
@@ -3816,7 +3838,7 @@
         <v>5</v>
       </c>
       <c r="P12" s="96"/>
-      <c r="Q12" s="94">
+      <c r="Q12" s="256">
         <f>(IF($Q11&lt;&gt;"",($Q$7*$O$40)+IF($Q$7=4,($O$38)+IF($Q11=$Q$7+$R$7,$O$39,0),0),0)+IF($R11&lt;&gt;"",($R$7*$O$40)+IF($R$7=4,($O$38)+IF($R11=$Q$7+$R$7,$O$39,0),0),0))</f>
         <v>5</v>
       </c>
@@ -3877,7 +3899,7 @@
 IF(D$7 = 4, 1, 0))</f>
         <v>1</v>
       </c>
-      <c r="E13" s="88">
+      <c r="E13" s="257">
         <f>IF(ISBLANK(E11),
 0,
 IF(E$7= 4, 1, 0))</f>
@@ -3949,7 +3971,7 @@
 IF(P$7 = 4, 1, 0))</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="102">
+      <c r="Q13" s="259">
         <f>IF(ISBLANK(Q11),
 0,
 IF(Q$7= 4, 1, 0))</f>
@@ -4070,7 +4092,7 @@
 IF(D11 = (C$7+D$7),1,0))</f>
         <v>1</v>
       </c>
-      <c r="E14" s="88">
+      <c r="E14" s="257">
         <f>IF(E13 = 0,
 0,
 IF(E11 = (E$7+F$7),1,0))</f>
@@ -4142,7 +4164,7 @@
 IF(P11 = (O$7+P$7),1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="102">
+      <c r="Q14" s="259">
         <f>IF(Q13 = 0,
 0,
 IF(Q11 = (Q$7+R$7),1,0))</f>
@@ -4284,7 +4306,7 @@
         <v>7</v>
       </c>
       <c r="P15" s="38"/>
-      <c r="Q15" s="147">
+      <c r="Q15" s="260">
         <v>6</v>
       </c>
       <c r="R15" s="43"/>
@@ -4807,7 +4829,7 @@
     <row r="19" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="148">
         <f>RANK(AL19,$AL$11:$AL$33,)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="149" t="s">
         <v>64</v>
@@ -5363,7 +5385,7 @@
     <row r="23" spans="1:38" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="87">
         <f>RANK(AL23,$AL$11:$AL$33,)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="65" t="s">
         <v>65</v>
@@ -5380,7 +5402,7 @@
       <c r="H23" s="40">
         <v>6</v>
       </c>
-      <c r="I23" s="37">
+      <c r="I23" s="253">
         <v>7</v>
       </c>
       <c r="J23" s="40"/>
@@ -5402,7 +5424,7 @@
       </c>
       <c r="S23" s="91">
         <f>SUM(C24:R24)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="T23" s="39"/>
       <c r="U23" s="40"/>
@@ -5432,11 +5454,11 @@
       </c>
       <c r="AK23" s="82">
         <f>MAX($AL$11:$AL$33) - AL23</f>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="AL23" s="91">
         <f>$S23+$AB23+$AG23+$AJ23</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:38" s="23" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5462,7 +5484,7 @@
       <c r="H24" s="110"/>
       <c r="I24" s="94">
         <f>(IF($I23&lt;&gt;"",($I$7*$O$40)+IF($I$7=4,($O$38)+IF($I23=$I$7+$J$7,$O$39,0),0),0)+IF($J23&lt;&gt;"",($J$7*$O$40)+IF($J$7=4,($O$38)+IF($J23=$I$7+$J$7,$O$39,0),0),0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J24" s="111"/>
       <c r="K24" s="112">
@@ -5573,7 +5595,7 @@
         <f>IF(ISBLANK(I23),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" s="88">
         <f>IF(ISBLANK(J23),
@@ -5719,7 +5741,7 @@
       <c r="AJ25" s="103"/>
       <c r="AK25" s="104">
         <f>SUM(C25:AI25)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL25" s="92"/>
     </row>
@@ -5766,7 +5788,7 @@
         <f>IF(I25 = 0,
 0,
 IF(I23 = (I$7+J$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="88">
         <f>IF(J25 = 0,
@@ -5912,7 +5934,7 @@
       <c r="AJ26" s="103"/>
       <c r="AK26" s="104">
         <f>SUM(C26:AI26)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL26" s="92"/>
     </row>
@@ -5932,7 +5954,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="162"/>
-      <c r="G27" s="254">
+      <c r="G27" s="188">
         <v>6</v>
       </c>
       <c r="H27" s="164"/>
@@ -5990,7 +6012,7 @@
         <f>MAX($AL$11:$AL$33) - AL27</f>
         <v>9</v>
       </c>
-      <c r="AL27" s="188">
+      <c r="AL27" s="187">
         <f>$S27+$AB27+$AG27+$AJ27</f>
         <v>17</v>
       </c>
@@ -6604,7 +6626,7 @@
         <f>IF(ISBLANK(#REF!),
 0,
 IF(I$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="88">
         <f>IF(ISBLANK(#REF!),
@@ -6750,7 +6772,7 @@
       <c r="AJ32" s="103"/>
       <c r="AK32" s="104">
         <f>SUM(C32:AI32)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AL32" s="92"/>
     </row>
@@ -6795,11 +6817,11 @@
 IF(#REF! = (G$7+H$7),1,0))</f>
         <v>0</v>
       </c>
-      <c r="I33" s="88">
+      <c r="I33" s="88" t="e">
         <f>IF(I32 = 0,
 0,
 IF(#REF! = (I$7+J$7),1,0))</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="J33" s="88">
         <f>IF(J32 = 0,
@@ -7082,12 +7104,12 @@
     <row r="36" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
       <c r="N36" s="22"/>
-      <c r="O36" s="226" t="s">
+      <c r="O36" s="238" t="s">
         <v>17</v>
       </c>
-      <c r="P36" s="227"/>
-      <c r="Q36" s="227"/>
-      <c r="R36" s="228"/>
+      <c r="P36" s="239"/>
+      <c r="Q36" s="239"/>
+      <c r="R36" s="240"/>
       <c r="AG36" s="25"/>
       <c r="AH36" s="25"/>
       <c r="AI36" s="25"/>
@@ -7096,21 +7118,21 @@
     </row>
     <row r="37" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
-      <c r="B37" s="216" t="s">
+      <c r="B37" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="217"/>
-      <c r="D37" s="217"/>
-      <c r="E37" s="217"/>
-      <c r="F37" s="217"/>
-      <c r="G37" s="217"/>
-      <c r="H37" s="217"/>
-      <c r="I37" s="217"/>
-      <c r="J37" s="217"/>
-      <c r="K37" s="217"/>
-      <c r="L37" s="217"/>
-      <c r="M37" s="217"/>
-      <c r="N37" s="218"/>
+      <c r="C37" s="229"/>
+      <c r="D37" s="229"/>
+      <c r="E37" s="229"/>
+      <c r="F37" s="229"/>
+      <c r="G37" s="229"/>
+      <c r="H37" s="229"/>
+      <c r="I37" s="229"/>
+      <c r="J37" s="229"/>
+      <c r="K37" s="229"/>
+      <c r="L37" s="229"/>
+      <c r="M37" s="229"/>
+      <c r="N37" s="230"/>
       <c r="O37" s="17">
         <v>1</v>
       </c>
@@ -7123,43 +7145,43 @@
       <c r="R37" s="18">
         <v>4</v>
       </c>
-      <c r="U37" s="229" t="s">
+      <c r="U37" s="241" t="s">
         <v>26</v>
       </c>
-      <c r="V37" s="230"/>
-      <c r="W37" s="230"/>
-      <c r="X37" s="230"/>
-      <c r="Y37" s="230"/>
-      <c r="Z37" s="230"/>
-      <c r="AA37" s="230"/>
-      <c r="AB37" s="230"/>
-      <c r="AC37" s="230"/>
-      <c r="AD37" s="231"/>
-      <c r="AG37" s="232" t="s">
+      <c r="V37" s="242"/>
+      <c r="W37" s="242"/>
+      <c r="X37" s="242"/>
+      <c r="Y37" s="242"/>
+      <c r="Z37" s="242"/>
+      <c r="AA37" s="242"/>
+      <c r="AB37" s="242"/>
+      <c r="AC37" s="242"/>
+      <c r="AD37" s="243"/>
+      <c r="AG37" s="244" t="s">
         <v>24</v>
       </c>
-      <c r="AH37" s="233"/>
-      <c r="AI37" s="233"/>
-      <c r="AJ37" s="233"/>
-      <c r="AK37" s="234"/>
+      <c r="AH37" s="245"/>
+      <c r="AI37" s="245"/>
+      <c r="AJ37" s="245"/>
+      <c r="AK37" s="246"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
-      <c r="B38" s="206" t="s">
+      <c r="B38" s="218" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="207"/>
-      <c r="D38" s="207"/>
-      <c r="E38" s="207"/>
-      <c r="F38" s="207"/>
-      <c r="G38" s="207"/>
-      <c r="H38" s="207"/>
-      <c r="I38" s="207"/>
-      <c r="J38" s="207"/>
-      <c r="K38" s="207"/>
-      <c r="L38" s="207"/>
-      <c r="M38" s="207"/>
-      <c r="N38" s="208"/>
+      <c r="C38" s="219"/>
+      <c r="D38" s="219"/>
+      <c r="E38" s="219"/>
+      <c r="F38" s="219"/>
+      <c r="G38" s="219"/>
+      <c r="H38" s="219"/>
+      <c r="I38" s="219"/>
+      <c r="J38" s="219"/>
+      <c r="K38" s="219"/>
+      <c r="L38" s="219"/>
+      <c r="M38" s="219"/>
+      <c r="N38" s="220"/>
       <c r="O38" s="16">
         <v>3</v>
       </c>
@@ -7172,49 +7194,49 @@
       <c r="R38" s="19">
         <v>3</v>
       </c>
-      <c r="U38" s="221" t="s">
+      <c r="U38" s="233" t="s">
         <v>20</v>
       </c>
-      <c r="V38" s="222"/>
-      <c r="W38" s="222"/>
-      <c r="X38" s="222"/>
-      <c r="Y38" s="222"/>
-      <c r="Z38" s="222"/>
-      <c r="AA38" s="222"/>
-      <c r="AB38" s="219">
+      <c r="V38" s="234"/>
+      <c r="W38" s="234"/>
+      <c r="X38" s="234"/>
+      <c r="Y38" s="234"/>
+      <c r="Z38" s="234"/>
+      <c r="AA38" s="234"/>
+      <c r="AB38" s="231">
         <v>5</v>
       </c>
-      <c r="AC38" s="219"/>
-      <c r="AD38" s="220"/>
+      <c r="AC38" s="231"/>
+      <c r="AD38" s="232"/>
       <c r="AE38" s="24"/>
       <c r="AF38" s="24"/>
-      <c r="AG38" s="235" t="s">
+      <c r="AG38" s="247" t="s">
         <v>21</v>
       </c>
-      <c r="AH38" s="236"/>
-      <c r="AI38" s="236"/>
-      <c r="AJ38" s="237"/>
+      <c r="AH38" s="248"/>
+      <c r="AI38" s="248"/>
+      <c r="AJ38" s="249"/>
       <c r="AK38" s="142">
         <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="206" t="s">
+      <c r="B39" s="218" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="207"/>
-      <c r="D39" s="207"/>
-      <c r="E39" s="207"/>
-      <c r="F39" s="207"/>
-      <c r="G39" s="207"/>
-      <c r="H39" s="207"/>
-      <c r="I39" s="207"/>
-      <c r="J39" s="207"/>
-      <c r="K39" s="207"/>
-      <c r="L39" s="207"/>
-      <c r="M39" s="207"/>
-      <c r="N39" s="208"/>
+      <c r="C39" s="219"/>
+      <c r="D39" s="219"/>
+      <c r="E39" s="219"/>
+      <c r="F39" s="219"/>
+      <c r="G39" s="219"/>
+      <c r="H39" s="219"/>
+      <c r="I39" s="219"/>
+      <c r="J39" s="219"/>
+      <c r="K39" s="219"/>
+      <c r="L39" s="219"/>
+      <c r="M39" s="219"/>
+      <c r="N39" s="220"/>
       <c r="O39" s="16">
         <v>2</v>
       </c>
@@ -7227,49 +7249,49 @@
       <c r="R39" s="19">
         <v>2</v>
       </c>
-      <c r="U39" s="211" t="s">
+      <c r="U39" s="223" t="s">
         <v>18</v>
       </c>
-      <c r="V39" s="212"/>
-      <c r="W39" s="212"/>
-      <c r="X39" s="212"/>
-      <c r="Y39" s="212"/>
-      <c r="Z39" s="212"/>
-      <c r="AA39" s="212"/>
-      <c r="AB39" s="239">
+      <c r="V39" s="224"/>
+      <c r="W39" s="224"/>
+      <c r="X39" s="224"/>
+      <c r="Y39" s="224"/>
+      <c r="Z39" s="224"/>
+      <c r="AA39" s="224"/>
+      <c r="AB39" s="251">
         <v>20</v>
       </c>
-      <c r="AC39" s="239"/>
-      <c r="AD39" s="240"/>
+      <c r="AC39" s="251"/>
+      <c r="AD39" s="252"/>
       <c r="AE39" s="24"/>
       <c r="AF39" s="24"/>
-      <c r="AG39" s="238" t="s">
+      <c r="AG39" s="250" t="s">
         <v>22</v>
       </c>
-      <c r="AH39" s="207"/>
-      <c r="AI39" s="207"/>
-      <c r="AJ39" s="208"/>
+      <c r="AH39" s="219"/>
+      <c r="AI39" s="219"/>
+      <c r="AJ39" s="220"/>
       <c r="AK39" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29"/>
-      <c r="B40" s="213" t="s">
+      <c r="B40" s="225" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="214"/>
-      <c r="D40" s="214"/>
-      <c r="E40" s="214"/>
-      <c r="F40" s="214"/>
-      <c r="G40" s="214"/>
-      <c r="H40" s="214"/>
-      <c r="I40" s="214"/>
-      <c r="J40" s="214"/>
-      <c r="K40" s="214"/>
-      <c r="L40" s="214"/>
-      <c r="M40" s="214"/>
-      <c r="N40" s="215"/>
+      <c r="C40" s="226"/>
+      <c r="D40" s="226"/>
+      <c r="E40" s="226"/>
+      <c r="F40" s="226"/>
+      <c r="G40" s="226"/>
+      <c r="H40" s="226"/>
+      <c r="I40" s="226"/>
+      <c r="J40" s="226"/>
+      <c r="K40" s="226"/>
+      <c r="L40" s="226"/>
+      <c r="M40" s="226"/>
+      <c r="N40" s="227"/>
       <c r="O40" s="3">
         <v>0</v>
       </c>
@@ -7282,51 +7304,51 @@
       <c r="R40" s="20">
         <v>0</v>
       </c>
-      <c r="U40" s="223" t="s">
+      <c r="U40" s="235" t="s">
         <v>19</v>
       </c>
-      <c r="V40" s="210"/>
-      <c r="W40" s="210"/>
-      <c r="X40" s="210"/>
-      <c r="Y40" s="210"/>
-      <c r="Z40" s="210"/>
-      <c r="AA40" s="210"/>
-      <c r="AB40" s="224">
+      <c r="V40" s="222"/>
+      <c r="W40" s="222"/>
+      <c r="X40" s="222"/>
+      <c r="Y40" s="222"/>
+      <c r="Z40" s="222"/>
+      <c r="AA40" s="222"/>
+      <c r="AB40" s="236">
         <f>AB38*AB39</f>
         <v>100</v>
       </c>
-      <c r="AC40" s="224"/>
-      <c r="AD40" s="225"/>
+      <c r="AC40" s="236"/>
+      <c r="AD40" s="237"/>
       <c r="AE40" s="24"/>
       <c r="AF40" s="24"/>
-      <c r="AG40" s="238" t="s">
+      <c r="AG40" s="250" t="s">
         <v>25</v>
       </c>
-      <c r="AH40" s="207"/>
-      <c r="AI40" s="207"/>
-      <c r="AJ40" s="208"/>
+      <c r="AH40" s="219"/>
+      <c r="AI40" s="219"/>
+      <c r="AJ40" s="220"/>
       <c r="AK40" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG41" s="211" t="s">
+      <c r="AG41" s="223" t="s">
         <v>23</v>
       </c>
-      <c r="AH41" s="212"/>
-      <c r="AI41" s="212"/>
-      <c r="AJ41" s="212"/>
+      <c r="AH41" s="224"/>
+      <c r="AI41" s="224"/>
+      <c r="AJ41" s="224"/>
       <c r="AK41" s="144">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG42" s="209" t="s">
+      <c r="AG42" s="221" t="s">
         <v>19</v>
       </c>
-      <c r="AH42" s="210"/>
-      <c r="AI42" s="210"/>
-      <c r="AJ42" s="210"/>
+      <c r="AH42" s="222"/>
+      <c r="AI42" s="222"/>
+      <c r="AJ42" s="222"/>
       <c r="AK42" s="143">
         <f>SUM(AK38:AK41)</f>
         <v>100</v>
@@ -7794,8 +7816,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8015,7 +8037,9 @@
       <c r="M6" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="64"/>
+      <c r="N6" s="64" t="s">
+        <v>41</v>
+      </c>
       <c r="O6" s="62"/>
       <c r="P6" s="62"/>
       <c r="Q6" s="62"/>
@@ -8072,7 +8096,9 @@
       <c r="M7" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="64"/>
+      <c r="N7" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="O7" s="62"/>
       <c r="P7" s="62"/>
       <c r="Q7" s="62"/>
@@ -8206,9 +8232,11 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="N10" s="64"/>
+        <v>30</v>
+      </c>
+      <c r="N10" s="64" t="s">
+        <v>55</v>
+      </c>
       <c r="O10" s="62"/>
       <c r="P10" s="62"/>
       <c r="Q10" s="62"/>
@@ -8264,9 +8292,11 @@
       </c>
       <c r="K11" s="13"/>
       <c r="M11" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="N11" s="64"/>
+        <v>31</v>
+      </c>
+      <c r="N11" s="64" t="s">
+        <v>57</v>
+      </c>
       <c r="O11" s="62"/>
       <c r="P11" s="62"/>
       <c r="Q11" s="62"/>
@@ -8345,10 +8375,12 @@
       <c r="H13" s="63">
         <v>2</v>
       </c>
-      <c r="I13" s="63"/>
+      <c r="I13" s="63">
+        <v>4</v>
+      </c>
       <c r="J13" s="61">
         <f>IF(C13&gt;C14,1,0)+IF(D13&gt;D14,1,0)+IF(E13&gt;E14,1,0)+IF(F13&gt;F14,1,0)+IF(G13&gt;G14,1,0)+IF(H13&gt;H14,1,0)+IF(I13&gt;I14,1,0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K13" s="15"/>
       <c r="M13" s="67"/>
@@ -8396,7 +8428,9 @@
       <c r="H14" s="63">
         <v>5</v>
       </c>
-      <c r="I14" s="63"/>
+      <c r="I14" s="63">
+        <v>0</v>
+      </c>
       <c r="J14" s="61">
         <f>IF(C14&gt;C13,1,0)+IF(D14&gt;D13,1,0)+IF(E14&gt;E13,1,0)+IF(F14&gt;F13,1,0)+IF(G14&gt;G13,1,0)+IF(H14&gt;H13,1,0)+IF(I14&gt;I13,1,0)</f>
         <v>3</v>
@@ -8673,9 +8707,11 @@
       <c r="K20" s="15"/>
       <c r="L20" s="12"/>
       <c r="M20" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="N20" s="64"/>
+        <v>37</v>
+      </c>
+      <c r="N20" s="64" t="s">
+        <v>51</v>
+      </c>
       <c r="O20" s="62"/>
       <c r="P20" s="62"/>
       <c r="Q20" s="62"/>
@@ -8733,7 +8769,9 @@
       <c r="M21" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="N21" s="64"/>
+      <c r="N21" s="64" t="s">
+        <v>59</v>
+      </c>
       <c r="O21" s="62"/>
       <c r="P21" s="62"/>
       <c r="Q21" s="62"/>
@@ -8865,9 +8903,11 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="N24" s="64"/>
+        <v>33</v>
+      </c>
+      <c r="N24" s="64" t="s">
+        <v>44</v>
+      </c>
       <c r="O24" s="62"/>
       <c r="P24" s="63"/>
       <c r="Q24" s="63"/>
@@ -8920,9 +8960,11 @@
       </c>
       <c r="K25" s="13"/>
       <c r="M25" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="N25" s="64"/>
+        <v>34</v>
+      </c>
+      <c r="N25" s="64" t="s">
+        <v>61</v>
+      </c>
       <c r="O25" s="62"/>
       <c r="P25" s="63"/>
       <c r="Q25" s="63"/>

</xml_diff>

<commit_message>
update start round 3
</commit_message>
<xml_diff>
--- a/chalet.xlsx
+++ b/chalet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F584C17-C3B2-4128-A689-38EB3CCFCDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5163A6-59C1-4EF8-AB1B-A017D0688785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="12495" windowWidth="28935" windowHeight="19185" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="12600" windowWidth="28935" windowHeight="19185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pool" sheetId="16" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <definedName name="PT_VICTOIRE_R4">Pool!$R$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>RONDE 1</t>
   </si>
@@ -1873,7 +1874,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="261">
+  <cellXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2102,18 +2103,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -2127,9 +2119,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2345,162 +2334,6 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2517,6 +2350,186 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="83" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="17" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="17" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="81" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="106" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3007,8 +3020,8 @@
   </sheetPr>
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AN50" sqref="AN50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3032,256 +3045,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="C1" s="214"/>
-      <c r="D1" s="214"/>
-      <c r="E1" s="214"/>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="214"/>
-      <c r="I1" s="214"/>
-      <c r="J1" s="214"/>
-      <c r="K1" s="214"/>
-      <c r="L1" s="214"/>
-      <c r="M1" s="214"/>
-      <c r="N1" s="214"/>
-      <c r="O1" s="214"/>
-      <c r="P1" s="215"/>
-      <c r="Q1" s="215"/>
-      <c r="R1" s="215"/>
-      <c r="S1" s="215"/>
-      <c r="T1" s="215"/>
-      <c r="U1" s="215"/>
-      <c r="V1" s="215"/>
-      <c r="W1" s="215"/>
-      <c r="X1" s="215"/>
-      <c r="Y1" s="215"/>
-      <c r="Z1" s="215"/>
-      <c r="AA1" s="215"/>
-      <c r="AB1" s="215"/>
-      <c r="AC1" s="215"/>
-      <c r="AD1" s="215"/>
-      <c r="AE1" s="215"/>
-      <c r="AF1" s="215"/>
-      <c r="AG1" s="215"/>
-      <c r="AH1" s="215"/>
-      <c r="AI1" s="215"/>
-      <c r="AJ1" s="215"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="255"/>
+      <c r="J1" s="255"/>
+      <c r="K1" s="255"/>
+      <c r="L1" s="255"/>
+      <c r="M1" s="255"/>
+      <c r="N1" s="255"/>
+      <c r="O1" s="255"/>
+      <c r="P1" s="256"/>
+      <c r="Q1" s="256"/>
+      <c r="R1" s="256"/>
+      <c r="S1" s="256"/>
+      <c r="T1" s="256"/>
+      <c r="U1" s="256"/>
+      <c r="V1" s="256"/>
+      <c r="W1" s="256"/>
+      <c r="X1" s="256"/>
+      <c r="Y1" s="256"/>
+      <c r="Z1" s="256"/>
+      <c r="AA1" s="256"/>
+      <c r="AB1" s="256"/>
+      <c r="AC1" s="256"/>
+      <c r="AD1" s="256"/>
+      <c r="AE1" s="256"/>
+      <c r="AF1" s="256"/>
+      <c r="AG1" s="256"/>
+      <c r="AH1" s="256"/>
+      <c r="AI1" s="256"/>
+      <c r="AJ1" s="256"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="34"/>
-      <c r="C2" s="216" t="s">
+      <c r="C2" s="257" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="216"/>
-      <c r="J2" s="216"/>
-      <c r="K2" s="216"/>
-      <c r="L2" s="216"/>
-      <c r="M2" s="216"/>
-      <c r="N2" s="216"/>
-      <c r="O2" s="216"/>
-      <c r="P2" s="216"/>
-      <c r="Q2" s="217" t="s">
+      <c r="D2" s="257"/>
+      <c r="E2" s="257"/>
+      <c r="F2" s="257"/>
+      <c r="G2" s="257"/>
+      <c r="H2" s="257"/>
+      <c r="I2" s="257"/>
+      <c r="J2" s="257"/>
+      <c r="K2" s="257"/>
+      <c r="L2" s="257"/>
+      <c r="M2" s="257"/>
+      <c r="N2" s="257"/>
+      <c r="O2" s="257"/>
+      <c r="P2" s="257"/>
+      <c r="Q2" s="258" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="215"/>
-      <c r="S2" s="215"/>
-      <c r="T2" s="215"/>
-      <c r="U2" s="215"/>
-      <c r="V2" s="215"/>
-      <c r="W2" s="215"/>
-      <c r="X2" s="215"/>
-      <c r="Y2" s="215"/>
-      <c r="Z2" s="215"/>
-      <c r="AA2" s="215"/>
-      <c r="AB2" s="215"/>
-      <c r="AC2" s="215"/>
-      <c r="AD2" s="215"/>
-      <c r="AE2" s="215"/>
-      <c r="AF2" s="215"/>
-      <c r="AG2" s="215"/>
-      <c r="AH2" s="215"/>
-      <c r="AI2" s="215"/>
-      <c r="AJ2" s="215"/>
+      <c r="R2" s="256"/>
+      <c r="S2" s="256"/>
+      <c r="T2" s="256"/>
+      <c r="U2" s="256"/>
+      <c r="V2" s="256"/>
+      <c r="W2" s="256"/>
+      <c r="X2" s="256"/>
+      <c r="Y2" s="256"/>
+      <c r="Z2" s="256"/>
+      <c r="AA2" s="256"/>
+      <c r="AB2" s="256"/>
+      <c r="AC2" s="256"/>
+      <c r="AD2" s="256"/>
+      <c r="AE2" s="256"/>
+      <c r="AF2" s="256"/>
+      <c r="AG2" s="256"/>
+      <c r="AH2" s="256"/>
+      <c r="AI2" s="256"/>
+      <c r="AJ2" s="256"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
-      <c r="C3" s="216" t="s">
+      <c r="C3" s="257" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
-      <c r="G3" s="216"/>
-      <c r="H3" s="216"/>
-      <c r="I3" s="216"/>
-      <c r="J3" s="216"/>
-      <c r="K3" s="216"/>
-      <c r="L3" s="216"/>
-      <c r="M3" s="216"/>
-      <c r="N3" s="216"/>
-      <c r="O3" s="216"/>
-      <c r="P3" s="216"/>
-      <c r="Q3" s="217" t="s">
+      <c r="D3" s="257"/>
+      <c r="E3" s="257"/>
+      <c r="F3" s="257"/>
+      <c r="G3" s="257"/>
+      <c r="H3" s="257"/>
+      <c r="I3" s="257"/>
+      <c r="J3" s="257"/>
+      <c r="K3" s="257"/>
+      <c r="L3" s="257"/>
+      <c r="M3" s="257"/>
+      <c r="N3" s="257"/>
+      <c r="O3" s="257"/>
+      <c r="P3" s="257"/>
+      <c r="Q3" s="258" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="215"/>
-      <c r="S3" s="215"/>
-      <c r="T3" s="215"/>
-      <c r="U3" s="215"/>
-      <c r="V3" s="215"/>
-      <c r="W3" s="215"/>
-      <c r="X3" s="215"/>
-      <c r="Y3" s="215"/>
-      <c r="Z3" s="215"/>
-      <c r="AA3" s="215"/>
-      <c r="AB3" s="215"/>
-      <c r="AC3" s="215"/>
-      <c r="AD3" s="215"/>
-      <c r="AE3" s="215"/>
-      <c r="AF3" s="215"/>
-      <c r="AG3" s="215"/>
-      <c r="AH3" s="215"/>
-      <c r="AI3" s="215"/>
-      <c r="AJ3" s="215"/>
+      <c r="R3" s="256"/>
+      <c r="S3" s="256"/>
+      <c r="T3" s="256"/>
+      <c r="U3" s="256"/>
+      <c r="V3" s="256"/>
+      <c r="W3" s="256"/>
+      <c r="X3" s="256"/>
+      <c r="Y3" s="256"/>
+      <c r="Z3" s="256"/>
+      <c r="AA3" s="256"/>
+      <c r="AB3" s="256"/>
+      <c r="AC3" s="256"/>
+      <c r="AD3" s="256"/>
+      <c r="AE3" s="256"/>
+      <c r="AF3" s="256"/>
+      <c r="AG3" s="256"/>
+      <c r="AH3" s="256"/>
+      <c r="AI3" s="256"/>
+      <c r="AJ3" s="256"/>
     </row>
     <row r="4" spans="1:38" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="214"/>
-      <c r="D4" s="214"/>
-      <c r="E4" s="214"/>
-      <c r="F4" s="214"/>
-      <c r="G4" s="214"/>
-      <c r="H4" s="214"/>
-      <c r="I4" s="214"/>
-      <c r="J4" s="214"/>
-      <c r="K4" s="214"/>
-      <c r="L4" s="214"/>
-      <c r="M4" s="214"/>
-      <c r="N4" s="214"/>
-      <c r="O4" s="214"/>
-      <c r="P4" s="215"/>
-      <c r="Q4" s="215"/>
-      <c r="R4" s="215"/>
-      <c r="S4" s="215"/>
-      <c r="T4" s="215"/>
-      <c r="U4" s="215"/>
-      <c r="V4" s="215"/>
-      <c r="W4" s="215"/>
-      <c r="X4" s="215"/>
-      <c r="Y4" s="215"/>
-      <c r="Z4" s="215"/>
-      <c r="AA4" s="215"/>
-      <c r="AB4" s="215"/>
-      <c r="AC4" s="215"/>
-      <c r="AD4" s="215"/>
-      <c r="AE4" s="215"/>
-      <c r="AF4" s="215"/>
-      <c r="AG4" s="215"/>
-      <c r="AH4" s="215"/>
-      <c r="AI4" s="215"/>
-      <c r="AJ4" s="215"/>
+      <c r="C4" s="255"/>
+      <c r="D4" s="255"/>
+      <c r="E4" s="255"/>
+      <c r="F4" s="255"/>
+      <c r="G4" s="255"/>
+      <c r="H4" s="255"/>
+      <c r="I4" s="255"/>
+      <c r="J4" s="255"/>
+      <c r="K4" s="255"/>
+      <c r="L4" s="255"/>
+      <c r="M4" s="255"/>
+      <c r="N4" s="255"/>
+      <c r="O4" s="255"/>
+      <c r="P4" s="256"/>
+      <c r="Q4" s="256"/>
+      <c r="R4" s="256"/>
+      <c r="S4" s="256"/>
+      <c r="T4" s="256"/>
+      <c r="U4" s="256"/>
+      <c r="V4" s="256"/>
+      <c r="W4" s="256"/>
+      <c r="X4" s="256"/>
+      <c r="Y4" s="256"/>
+      <c r="Z4" s="256"/>
+      <c r="AA4" s="256"/>
+      <c r="AB4" s="256"/>
+      <c r="AC4" s="256"/>
+      <c r="AD4" s="256"/>
+      <c r="AE4" s="256"/>
+      <c r="AF4" s="256"/>
+      <c r="AG4" s="256"/>
+      <c r="AH4" s="256"/>
+      <c r="AI4" s="256"/>
+      <c r="AJ4" s="256"/>
     </row>
     <row r="5" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="201" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="202"/>
-      <c r="E5" s="202"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="202"/>
-      <c r="H5" s="202"/>
-      <c r="I5" s="202"/>
-      <c r="J5" s="202"/>
-      <c r="K5" s="202"/>
-      <c r="L5" s="202"/>
-      <c r="M5" s="202"/>
-      <c r="N5" s="202"/>
-      <c r="O5" s="202"/>
-      <c r="P5" s="202"/>
-      <c r="Q5" s="202"/>
-      <c r="R5" s="202"/>
-      <c r="S5" s="203"/>
-      <c r="T5" s="201" t="s">
+      <c r="C5" s="259" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="260"/>
+      <c r="E5" s="260"/>
+      <c r="F5" s="260"/>
+      <c r="G5" s="260"/>
+      <c r="H5" s="260"/>
+      <c r="I5" s="260"/>
+      <c r="J5" s="260"/>
+      <c r="K5" s="260"/>
+      <c r="L5" s="260"/>
+      <c r="M5" s="260"/>
+      <c r="N5" s="260"/>
+      <c r="O5" s="260"/>
+      <c r="P5" s="260"/>
+      <c r="Q5" s="260"/>
+      <c r="R5" s="260"/>
+      <c r="S5" s="261"/>
+      <c r="T5" s="259" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="202"/>
-      <c r="V5" s="202"/>
-      <c r="W5" s="202"/>
-      <c r="X5" s="202"/>
-      <c r="Y5" s="202"/>
-      <c r="Z5" s="202"/>
-      <c r="AA5" s="202"/>
-      <c r="AB5" s="203"/>
-      <c r="AC5" s="201" t="s">
+      <c r="U5" s="260"/>
+      <c r="V5" s="260"/>
+      <c r="W5" s="260"/>
+      <c r="X5" s="260"/>
+      <c r="Y5" s="260"/>
+      <c r="Z5" s="260"/>
+      <c r="AA5" s="260"/>
+      <c r="AB5" s="261"/>
+      <c r="AC5" s="259" t="s">
         <v>2</v>
       </c>
-      <c r="AD5" s="202"/>
-      <c r="AE5" s="202"/>
-      <c r="AF5" s="202"/>
-      <c r="AG5" s="204"/>
-      <c r="AH5" s="201" t="s">
+      <c r="AD5" s="260"/>
+      <c r="AE5" s="260"/>
+      <c r="AF5" s="260"/>
+      <c r="AG5" s="262"/>
+      <c r="AH5" s="259" t="s">
         <v>10</v>
       </c>
-      <c r="AI5" s="202"/>
-      <c r="AJ5" s="203"/>
+      <c r="AI5" s="260"/>
+      <c r="AJ5" s="261"/>
     </row>
     <row r="6" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="205" t="s">
+      <c r="C6" s="232" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="206"/>
-      <c r="E6" s="206"/>
-      <c r="F6" s="206"/>
-      <c r="G6" s="206"/>
-      <c r="H6" s="206"/>
-      <c r="I6" s="206"/>
-      <c r="J6" s="207"/>
-      <c r="K6" s="212" t="s">
+      <c r="D6" s="227"/>
+      <c r="E6" s="227"/>
+      <c r="F6" s="227"/>
+      <c r="G6" s="227"/>
+      <c r="H6" s="227"/>
+      <c r="I6" s="227"/>
+      <c r="J6" s="228"/>
+      <c r="K6" s="226" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="206"/>
-      <c r="M6" s="206"/>
-      <c r="N6" s="206"/>
-      <c r="O6" s="206"/>
-      <c r="P6" s="206"/>
-      <c r="Q6" s="206"/>
-      <c r="R6" s="207"/>
-      <c r="S6" s="208" t="s">
+      <c r="L6" s="227"/>
+      <c r="M6" s="227"/>
+      <c r="N6" s="227"/>
+      <c r="O6" s="227"/>
+      <c r="P6" s="227"/>
+      <c r="Q6" s="227"/>
+      <c r="R6" s="228"/>
+      <c r="S6" s="229" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="205" t="s">
+      <c r="T6" s="232" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="206"/>
-      <c r="V6" s="206"/>
-      <c r="W6" s="207"/>
-      <c r="X6" s="212" t="s">
+      <c r="U6" s="227"/>
+      <c r="V6" s="227"/>
+      <c r="W6" s="228"/>
+      <c r="X6" s="226" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="206"/>
-      <c r="Z6" s="206"/>
-      <c r="AA6" s="207"/>
-      <c r="AB6" s="208" t="s">
+      <c r="Y6" s="227"/>
+      <c r="Z6" s="227"/>
+      <c r="AA6" s="228"/>
+      <c r="AB6" s="229" t="s">
         <v>13</v>
       </c>
-      <c r="AC6" s="213" t="s">
+      <c r="AC6" s="264" t="s">
         <v>9</v>
       </c>
-      <c r="AD6" s="207"/>
-      <c r="AE6" s="212" t="s">
+      <c r="AD6" s="228"/>
+      <c r="AE6" s="226" t="s">
         <v>8</v>
       </c>
-      <c r="AF6" s="207"/>
-      <c r="AG6" s="208" t="s">
+      <c r="AF6" s="228"/>
+      <c r="AG6" s="229" t="s">
         <v>14</v>
       </c>
       <c r="AH6" s="46"/>
       <c r="AI6" s="21"/>
-      <c r="AJ6" s="208" t="s">
+      <c r="AJ6" s="229" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3291,11 +3304,11 @@
         <f>Résultats!$J$3</f>
         <v>3</v>
       </c>
-      <c r="D7" s="189">
+      <c r="D7" s="185">
         <f>Résultats!$J$4</f>
         <v>4</v>
       </c>
-      <c r="E7" s="193">
+      <c r="E7" s="189">
         <f>Résultats!$J$6</f>
         <v>4</v>
       </c>
@@ -3303,7 +3316,7 @@
         <f>Résultats!$J$7</f>
         <v>2</v>
       </c>
-      <c r="G7" s="193">
+      <c r="G7" s="189">
         <f>Résultats!$J$10</f>
         <v>4</v>
       </c>
@@ -3311,7 +3324,7 @@
         <f>Résultats!$J$11</f>
         <v>2</v>
       </c>
-      <c r="I7" s="193">
+      <c r="I7" s="189">
         <f>Résultats!$J$13</f>
         <v>4</v>
       </c>
@@ -3323,11 +3336,11 @@
         <f>Résultats!$J$17</f>
         <v>3</v>
       </c>
-      <c r="L7" s="189">
+      <c r="L7" s="185">
         <f>Résultats!$J$18</f>
         <v>4</v>
       </c>
-      <c r="M7" s="193">
+      <c r="M7" s="189">
         <f>Résultats!$J$20</f>
         <v>4</v>
       </c>
@@ -3335,7 +3348,7 @@
         <f>Résultats!$J$21</f>
         <v>2</v>
       </c>
-      <c r="O7" s="193">
+      <c r="O7" s="189">
         <f>Résultats!$J$24</f>
         <v>4</v>
       </c>
@@ -3343,7 +3356,7 @@
         <f>Résultats!$J$25</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="200">
+      <c r="Q7" s="196">
         <f>Résultats!$J$27</f>
         <v>4</v>
       </c>
@@ -3351,41 +3364,41 @@
         <f>Résultats!$J$28</f>
         <v>2</v>
       </c>
-      <c r="S7" s="209"/>
-      <c r="T7" s="115">
+      <c r="S7" s="230"/>
+      <c r="T7" s="205">
         <f>Résultats!$V$6</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U7" s="76">
         <f>Résultats!$V$7</f>
-        <v>0</v>
-      </c>
-      <c r="V7" s="118">
+        <v>1</v>
+      </c>
+      <c r="V7" s="189">
         <f>Résultats!$V$10</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W7" s="76">
         <f>Résultats!$V$11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7" s="78">
         <f>Résultats!$V$20</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="77">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="209">
         <f>Résultats!$V$21</f>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="186">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="196">
         <f>Résultats!$V$24</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA7" s="76">
         <f>Résultats!$V$25</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="209"/>
-      <c r="AC7" s="186">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="230"/>
+      <c r="AC7" s="182">
         <f>Résultats!$AH$8</f>
         <v>0</v>
       </c>
@@ -3401,8 +3414,8 @@
         <f>Résultats!$AH$23</f>
         <v>0</v>
       </c>
-      <c r="AG7" s="209"/>
-      <c r="AH7" s="132">
+      <c r="AG7" s="230"/>
+      <c r="AH7" s="128">
         <f>Résultats!$AH$15</f>
         <v>0</v>
       </c>
@@ -3410,7 +3423,7 @@
         <f>Résultats!$AH$16</f>
         <v>0</v>
       </c>
-      <c r="AJ7" s="209"/>
+      <c r="AJ7" s="230"/>
     </row>
     <row r="8" spans="1:38" s="31" customFormat="1" ht="58.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32"/>
@@ -3419,39 +3432,39 @@
 +IF(ISBLANK($D11),0,($D$7*PT_VICTOIRE_R1)+IF($D$7=4,PT_PREDICTION_EQUIPE_R1+IF($D11=$C$7+$D$7,PT_PREDICTION_NB_PARTIES_R1,0),0))</f>
         <v>5</v>
       </c>
-      <c r="D8" s="190"/>
-      <c r="E8" s="194"/>
+      <c r="D8" s="186"/>
+      <c r="E8" s="190"/>
       <c r="F8" s="84"/>
-      <c r="G8" s="197"/>
+      <c r="G8" s="193"/>
       <c r="H8" s="83"/>
-      <c r="I8" s="194"/>
+      <c r="I8" s="190"/>
       <c r="J8" s="83"/>
       <c r="K8" s="86"/>
-      <c r="L8" s="190"/>
-      <c r="M8" s="194"/>
+      <c r="L8" s="186"/>
+      <c r="M8" s="190"/>
       <c r="N8" s="84"/>
-      <c r="O8" s="194"/>
+      <c r="O8" s="190"/>
       <c r="P8" s="84"/>
-      <c r="Q8" s="197"/>
+      <c r="Q8" s="193"/>
       <c r="R8" s="83"/>
-      <c r="S8" s="209"/>
-      <c r="T8" s="116"/>
+      <c r="S8" s="230"/>
+      <c r="T8" s="206"/>
       <c r="U8" s="83"/>
-      <c r="V8" s="119"/>
+      <c r="V8" s="190"/>
       <c r="W8" s="83"/>
       <c r="X8" s="86"/>
-      <c r="Y8" s="84"/>
-      <c r="Z8" s="85"/>
+      <c r="Y8" s="210"/>
+      <c r="Z8" s="193"/>
       <c r="AA8" s="83"/>
-      <c r="AB8" s="209"/>
+      <c r="AB8" s="230"/>
       <c r="AC8" s="85"/>
       <c r="AD8" s="83"/>
       <c r="AE8" s="86"/>
       <c r="AF8" s="83"/>
-      <c r="AG8" s="209"/>
-      <c r="AH8" s="132"/>
+      <c r="AG8" s="230"/>
+      <c r="AH8" s="128"/>
       <c r="AI8" s="79"/>
-      <c r="AJ8" s="209"/>
+      <c r="AJ8" s="230"/>
     </row>
     <row r="9" spans="1:38" s="31" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32"/>
@@ -3459,126 +3472,126 @@
         <f>Résultats!$B$3</f>
         <v>BOSTON</v>
       </c>
-      <c r="D9" s="191" t="str">
+      <c r="D9" s="187" t="str">
         <f>Résultats!$B$4</f>
         <v>FLORIDA</v>
       </c>
-      <c r="E9" s="195" t="str">
+      <c r="E9" s="191" t="str">
         <f>Résultats!$B$6</f>
         <v>TORONTO</v>
       </c>
-      <c r="F9" s="122" t="str">
+      <c r="F9" s="119" t="str">
         <f>Résultats!$B$7</f>
         <v>TAMPA BAY</v>
       </c>
-      <c r="G9" s="198" t="str">
+      <c r="G9" s="194" t="str">
         <f>Résultats!$B$10</f>
         <v>CAROLINA</v>
       </c>
-      <c r="H9" s="120" t="str">
+      <c r="H9" s="118" t="str">
         <f>Résultats!$B$11</f>
         <v>NY ISLANDERS</v>
       </c>
-      <c r="I9" s="195" t="str">
+      <c r="I9" s="191" t="str">
         <f>Résultats!$B$13</f>
         <v>NEW JERSEY</v>
       </c>
-      <c r="J9" s="120" t="str">
+      <c r="J9" s="118" t="str">
         <f>Résultats!$B$14</f>
         <v>NY RANGERS</v>
       </c>
-      <c r="K9" s="124" t="str">
+      <c r="K9" s="121" t="str">
         <f>Résultats!$B$17</f>
         <v>COLORADO</v>
       </c>
-      <c r="L9" s="191" t="str">
+      <c r="L9" s="187" t="str">
         <f>Résultats!$B$18</f>
         <v>SEATTLE</v>
       </c>
-      <c r="M9" s="195" t="str">
+      <c r="M9" s="191" t="str">
         <f>Résultats!$B$20</f>
         <v>DALLAS</v>
       </c>
-      <c r="N9" s="122" t="str">
+      <c r="N9" s="119" t="str">
         <f>Résultats!$B$21</f>
         <v>MINNESOTA</v>
       </c>
-      <c r="O9" s="195" t="str">
+      <c r="O9" s="191" t="str">
         <f>Résultats!$B$24</f>
         <v>VEGAS</v>
       </c>
-      <c r="P9" s="122" t="str">
+      <c r="P9" s="119" t="str">
         <f>Résultats!$B$25</f>
         <v>WINNIPEG</v>
       </c>
-      <c r="Q9" s="198" t="str">
+      <c r="Q9" s="194" t="str">
         <f>Résultats!$B$27</f>
         <v>EDMONTON</v>
       </c>
-      <c r="R9" s="120" t="str">
+      <c r="R9" s="118" t="str">
         <f>Résultats!$B$28</f>
         <v>LOS ANGELES</v>
       </c>
-      <c r="S9" s="209"/>
-      <c r="T9" s="117" t="str">
+      <c r="S9" s="230"/>
+      <c r="T9" s="207" t="str">
         <f>Résultats!$N$6</f>
+        <v>FLORIDA</v>
+      </c>
+      <c r="U9" s="118" t="str">
+        <f>Résultats!$N$7</f>
         <v>TORONTO</v>
       </c>
-      <c r="U9" s="120" t="str">
-        <f>Résultats!$N$7</f>
-        <v>FLORIDA</v>
-      </c>
-      <c r="V9" s="121" t="str">
+      <c r="V9" s="191" t="str">
         <f>Résultats!$N$10</f>
         <v>CAROLINA</v>
       </c>
-      <c r="W9" s="120" t="str">
+      <c r="W9" s="118" t="str">
         <f>Résultats!$N$11</f>
         <v>NEW JERSEY</v>
       </c>
-      <c r="X9" s="124" t="str">
+      <c r="X9" s="121" t="str">
         <f>Résultats!$N$20</f>
+        <v>SEATTLE</v>
+      </c>
+      <c r="Y9" s="211" t="str">
+        <f>Résultats!$N$21</f>
         <v>DALLAS</v>
       </c>
-      <c r="Y9" s="122" t="str">
-        <f>Résultats!$N$21</f>
-        <v>SEATTLE</v>
-      </c>
-      <c r="Z9" s="123" t="str">
+      <c r="Z9" s="194" t="str">
         <f>Résultats!$N$24</f>
         <v>VEGAS</v>
       </c>
-      <c r="AA9" s="120" t="str">
+      <c r="AA9" s="118" t="str">
         <f>Résultats!$N$25</f>
         <v>EDMONTON</v>
       </c>
-      <c r="AB9" s="209"/>
-      <c r="AC9" s="123">
+      <c r="AB9" s="230"/>
+      <c r="AC9" s="120" t="str">
         <f>Résultats!$Z$8</f>
-        <v>0</v>
-      </c>
-      <c r="AD9" s="120">
+        <v>FLORIDA</v>
+      </c>
+      <c r="AD9" s="118" t="str">
         <f>Résultats!$Z$9</f>
-        <v>0</v>
-      </c>
-      <c r="AE9" s="124">
+        <v>CAROLINA</v>
+      </c>
+      <c r="AE9" s="121" t="str">
         <f>Résultats!$Z$22</f>
-        <v>0</v>
-      </c>
-      <c r="AF9" s="120">
+        <v>DALLAS</v>
+      </c>
+      <c r="AF9" s="118" t="str">
         <f>Résultats!$Z$23</f>
-        <v>0</v>
-      </c>
-      <c r="AG9" s="209"/>
-      <c r="AH9" s="133">
+        <v>VEGAS</v>
+      </c>
+      <c r="AG9" s="230"/>
+      <c r="AH9" s="129">
         <f>Résultats!$Z$15</f>
         <v>0</v>
       </c>
-      <c r="AI9" s="134">
+      <c r="AI9" s="130">
         <f>Résultats!$Z$16</f>
         <v>0</v>
       </c>
-      <c r="AJ9" s="209"/>
+      <c r="AJ9" s="230"/>
     </row>
     <row r="10" spans="1:38" s="31" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
@@ -3587,130 +3600,130 @@
       <c r="B10" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="125" t="str">
+      <c r="C10" s="122" t="str">
         <f>Résultats!$A$3</f>
         <v>A1</v>
       </c>
-      <c r="D10" s="192" t="str">
+      <c r="D10" s="188" t="str">
         <f>Résultats!$A$4</f>
         <v>WC2</v>
       </c>
-      <c r="E10" s="196" t="str">
+      <c r="E10" s="192" t="str">
         <f>Résultats!$A$6</f>
         <v>A2</v>
       </c>
-      <c r="F10" s="128" t="str">
+      <c r="F10" s="124" t="str">
         <f>Résultats!$A$7</f>
         <v>A3</v>
       </c>
-      <c r="G10" s="199" t="str">
+      <c r="G10" s="195" t="str">
         <f>Résultats!$A$10</f>
         <v>M1</v>
       </c>
-      <c r="H10" s="126" t="str">
+      <c r="H10" s="123" t="str">
         <f>Résultats!$A$11</f>
         <v>WC1</v>
       </c>
-      <c r="I10" s="196" t="str">
+      <c r="I10" s="192" t="str">
         <f>Résultats!$A$13</f>
         <v>M2</v>
       </c>
-      <c r="J10" s="126" t="str">
+      <c r="J10" s="123" t="str">
         <f>Résultats!$A$14</f>
         <v>M3</v>
       </c>
-      <c r="K10" s="130" t="str">
+      <c r="K10" s="126" t="str">
         <f>Résultats!$A$17</f>
         <v>C1</v>
       </c>
-      <c r="L10" s="192" t="str">
+      <c r="L10" s="188" t="str">
         <f>Résultats!$A$18</f>
         <v>WC2</v>
       </c>
-      <c r="M10" s="196" t="str">
+      <c r="M10" s="192" t="str">
         <f>Résultats!$A$20</f>
         <v>C2</v>
       </c>
-      <c r="N10" s="128" t="str">
+      <c r="N10" s="124" t="str">
         <f>Résultats!$A$21</f>
         <v>C3</v>
       </c>
-      <c r="O10" s="196" t="str">
+      <c r="O10" s="192" t="str">
         <f>Résultats!$A$24</f>
         <v>P1</v>
       </c>
-      <c r="P10" s="128" t="str">
+      <c r="P10" s="124" t="str">
         <f>Résultats!$A$25</f>
         <v>WC1</v>
       </c>
-      <c r="Q10" s="199" t="str">
+      <c r="Q10" s="195" t="str">
         <f>Résultats!$A$27</f>
         <v>P2</v>
       </c>
-      <c r="R10" s="131" t="str">
+      <c r="R10" s="127" t="str">
         <f>Résultats!$A$28</f>
         <v>P3</v>
       </c>
-      <c r="S10" s="211"/>
-      <c r="T10" s="125" t="str">
+      <c r="S10" s="231"/>
+      <c r="T10" s="208" t="str">
         <f>Résultats!$M$6</f>
+        <v>WC2</v>
+      </c>
+      <c r="U10" s="123" t="str">
+        <f>Résultats!$M$7</f>
         <v>A2</v>
       </c>
-      <c r="U10" s="126" t="str">
-        <f>Résultats!$M$7</f>
-        <v>WC2</v>
-      </c>
-      <c r="V10" s="127" t="str">
+      <c r="V10" s="192" t="str">
         <f>Résultats!$M$10</f>
         <v>M1</v>
       </c>
-      <c r="W10" s="126" t="str">
+      <c r="W10" s="123" t="str">
         <f>Résultats!$M$11</f>
         <v>M2</v>
       </c>
-      <c r="X10" s="130" t="str">
+      <c r="X10" s="126" t="str">
         <f>Résultats!$M$20</f>
+        <v>WC2</v>
+      </c>
+      <c r="Y10" s="212" t="str">
+        <f>Résultats!$M$21</f>
         <v>C2</v>
       </c>
-      <c r="Y10" s="128" t="str">
-        <f>Résultats!$M$21</f>
-        <v>WC2</v>
-      </c>
-      <c r="Z10" s="129" t="str">
+      <c r="Z10" s="195" t="str">
         <f>Résultats!$M$24</f>
         <v>P1</v>
       </c>
-      <c r="AA10" s="131" t="str">
+      <c r="AA10" s="127" t="str">
         <f>Résultats!$M$25</f>
         <v>P2</v>
       </c>
-      <c r="AB10" s="210"/>
-      <c r="AC10" s="129" t="str">
+      <c r="AB10" s="263"/>
+      <c r="AC10" s="125" t="str">
         <f>Résultats!$Y$8</f>
-        <v>A2</v>
-      </c>
-      <c r="AD10" s="126" t="str">
+        <v>WC2</v>
+      </c>
+      <c r="AD10" s="123" t="str">
         <f>Résultats!$Y$9</f>
-        <v>WC1</v>
-      </c>
-      <c r="AE10" s="130" t="str">
+        <v>M1</v>
+      </c>
+      <c r="AE10" s="126" t="str">
         <f>Résultats!$Y$22</f>
-        <v>P2</v>
-      </c>
-      <c r="AF10" s="126" t="str">
+        <v>C2</v>
+      </c>
+      <c r="AF10" s="123" t="str">
         <f>Résultats!$Y$23</f>
-        <v>C3</v>
-      </c>
-      <c r="AG10" s="210"/>
-      <c r="AH10" s="135" t="str">
+        <v>P1</v>
+      </c>
+      <c r="AG10" s="263"/>
+      <c r="AH10" s="131" t="str">
         <f>Résultats!$Y$15</f>
         <v>A2</v>
       </c>
-      <c r="AI10" s="136" t="str">
+      <c r="AI10" s="132" t="str">
         <f>Résultats!$Y$16</f>
         <v>C3</v>
       </c>
-      <c r="AJ10" s="211"/>
+      <c r="AJ10" s="231"/>
       <c r="AK10" s="81" t="s">
         <v>46</v>
       </c>
@@ -3719,82 +3732,94 @@
       </c>
     </row>
     <row r="11" spans="1:38" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="148">
+      <c r="A11" s="144">
         <f>RANK(AL11,$AL$11:$AL$33,)</f>
         <v>1</v>
       </c>
-      <c r="B11" s="149" t="s">
+      <c r="B11" s="145" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="150"/>
-      <c r="D11" s="254">
+      <c r="C11" s="146"/>
+      <c r="D11" s="198">
         <v>7</v>
       </c>
-      <c r="E11" s="255">
+      <c r="E11" s="199">
         <v>6</v>
       </c>
-      <c r="F11" s="151"/>
-      <c r="G11" s="153">
+      <c r="F11" s="147"/>
+      <c r="G11" s="149">
         <v>5</v>
       </c>
-      <c r="H11" s="154"/>
-      <c r="I11" s="152"/>
-      <c r="J11" s="154">
+      <c r="H11" s="150"/>
+      <c r="I11" s="148"/>
+      <c r="J11" s="150">
         <v>7</v>
       </c>
-      <c r="K11" s="155">
+      <c r="K11" s="151">
         <v>6</v>
       </c>
-      <c r="L11" s="154"/>
-      <c r="M11" s="152">
+      <c r="L11" s="150"/>
+      <c r="M11" s="148">
         <v>7</v>
       </c>
-      <c r="N11" s="182"/>
-      <c r="O11" s="255">
+      <c r="N11" s="178"/>
+      <c r="O11" s="199">
         <v>5</v>
       </c>
-      <c r="P11" s="151"/>
-      <c r="Q11" s="258">
+      <c r="P11" s="147"/>
+      <c r="Q11" s="202">
         <v>6</v>
       </c>
-      <c r="R11" s="156"/>
-      <c r="S11" s="157">
+      <c r="R11" s="152"/>
+      <c r="S11" s="153">
         <f>SUM(C12:R12)</f>
         <v>26</v>
       </c>
-      <c r="T11" s="183"/>
-      <c r="U11" s="154"/>
-      <c r="V11" s="152"/>
-      <c r="W11" s="154"/>
-      <c r="X11" s="155"/>
-      <c r="Y11" s="151"/>
-      <c r="Z11" s="153"/>
-      <c r="AA11" s="156"/>
-      <c r="AB11" s="157">
+      <c r="T11" s="179"/>
+      <c r="U11" s="150">
+        <v>6</v>
+      </c>
+      <c r="V11" s="148">
+        <v>7</v>
+      </c>
+      <c r="W11" s="150"/>
+      <c r="X11" s="151"/>
+      <c r="Y11" s="147">
+        <v>6</v>
+      </c>
+      <c r="Z11" s="149">
+        <v>7</v>
+      </c>
+      <c r="AA11" s="152"/>
+      <c r="AB11" s="153">
         <f>SUM(T12:AA12)</f>
-        <v>0</v>
-      </c>
-      <c r="AC11" s="153"/>
-      <c r="AD11" s="154"/>
-      <c r="AE11" s="155"/>
-      <c r="AF11" s="154"/>
-      <c r="AG11" s="157">
+        <v>9</v>
+      </c>
+      <c r="AC11" s="149"/>
+      <c r="AD11" s="150">
+        <v>6</v>
+      </c>
+      <c r="AE11" s="151">
+        <v>6</v>
+      </c>
+      <c r="AF11" s="150"/>
+      <c r="AG11" s="153">
         <f>SUM(AC12:AF12)</f>
         <v>0</v>
       </c>
-      <c r="AH11" s="184"/>
-      <c r="AI11" s="185"/>
-      <c r="AJ11" s="157">
+      <c r="AH11" s="180"/>
+      <c r="AI11" s="181"/>
+      <c r="AJ11" s="153">
         <f>AH12</f>
         <v>0</v>
       </c>
-      <c r="AK11" s="160">
+      <c r="AK11" s="156">
         <f>MAX($AL$11:$AL$33) - AL11</f>
         <v>0</v>
       </c>
-      <c r="AL11" s="157">
+      <c r="AL11" s="153">
         <f>$S11+$AB11+$AG11+$AJ11</f>
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:38" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -3808,7 +3833,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="96"/>
-      <c r="E12" s="256">
+      <c r="E12" s="200">
         <f>(IF($E11&lt;&gt;"",($E$7*$O$40)+IF($E$7=4,($O$38)+IF($E11=$E$7+$F$7,$O$39,0),0),0)+IF($F11&lt;&gt;"",($F$7*$O$40)+IF($F$7=4,($O$38)+IF($F11=$E$7+$F$7,$O$39,0),0),0))</f>
         <v>5</v>
       </c>
@@ -3838,7 +3863,7 @@
         <v>5</v>
       </c>
       <c r="P12" s="96"/>
-      <c r="Q12" s="256">
+      <c r="Q12" s="200">
         <f>(IF($Q11&lt;&gt;"",($Q$7*$O$40)+IF($Q$7=4,($O$38)+IF($Q11=$Q$7+$R$7,$O$39,0),0),0)+IF($R11&lt;&gt;"",($R$7*$O$40)+IF($R$7=4,($O$38)+IF($R11=$Q$7+$R$7,$O$39,0),0),0))</f>
         <v>5</v>
       </c>
@@ -3851,17 +3876,17 @@
       <c r="U12" s="95"/>
       <c r="V12" s="95">
         <f>(IF($V11&lt;&gt;"",($V$7*$P$40)+IF($V$7=4,($P$38)+IF($V11=$V$7+$W$7,$P$39,0),0),0)+IF($W11&lt;&gt;"",($W$7*$P$40)+IF($W$7=4,($P$38)+IF($W11=$V$7+$W$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W12" s="95"/>
       <c r="X12" s="95">
         <f>(IF($X11&lt;&gt;"",($X$7*$P$40)+IF($X$7=4,($P$38)+IF($X11=$X$7+$Y$7,$P$39,0),0),0)+IF($Y11&lt;&gt;"",($Y$7*$P$40)+IF($Y$7=4,($P$38)+IF($Y11=$X$7+$Y$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y12" s="49"/>
       <c r="Z12" s="95">
         <f>(IF($Z11&lt;&gt;"",($Z$7*$P$40)+IF($Z$7=4,($P$38)+IF($Z11=$Z$7+$AA$7,$P$39,0),0),0)+IF($AA11&lt;&gt;"",($AA$7*$P$40)+IF($AA$7=4,($P$38)+IF($AA11=$Z$7+$AA$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA12" s="50"/>
       <c r="AB12" s="90"/>
@@ -3899,7 +3924,7 @@
 IF(D$7 = 4, 1, 0))</f>
         <v>1</v>
       </c>
-      <c r="E13" s="257">
+      <c r="E13" s="201">
         <f>IF(ISBLANK(E11),
 0,
 IF(E$7= 4, 1, 0))</f>
@@ -3971,7 +3996,7 @@
 IF(P$7 = 4, 1, 0))</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="259">
+      <c r="Q13" s="203">
         <f>IF(ISBLANK(Q11),
 0,
 IF(Q$7= 4, 1, 0))</f>
@@ -4000,7 +4025,7 @@
         <f>IF(ISBLANK(V11),
 0,
 IF(V$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="88">
         <f>IF(ISBLANK(W11),
@@ -4018,13 +4043,13 @@
         <f>IF(ISBLANK(Y11),
 0,
 IF(Y$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13" s="88">
         <f>IF(ISBLANK(Z11),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA13" s="88">
         <f>IF(ISBLANK(AA11),
@@ -4073,7 +4098,7 @@
       <c r="AJ13" s="103"/>
       <c r="AK13" s="104">
         <f>SUM(C13:AI13)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AL13" s="92"/>
     </row>
@@ -4092,7 +4117,7 @@
 IF(D11 = (C$7+D$7),1,0))</f>
         <v>1</v>
       </c>
-      <c r="E14" s="257">
+      <c r="E14" s="201">
         <f>IF(E13 = 0,
 0,
 IF(E11 = (E$7+F$7),1,0))</f>
@@ -4164,7 +4189,7 @@
 IF(P11 = (O$7+P$7),1,0))</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="259">
+      <c r="Q14" s="203">
         <f>IF(Q13 = 0,
 0,
 IF(Q11 = (Q$7+R$7),1,0))</f>
@@ -4282,7 +4307,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="38"/>
-      <c r="E15" s="253">
+      <c r="E15" s="197">
         <v>6</v>
       </c>
       <c r="F15" s="38"/>
@@ -4298,15 +4323,15 @@
         <v>6</v>
       </c>
       <c r="L15" s="40"/>
-      <c r="M15" s="253">
+      <c r="M15" s="197">
         <v>6</v>
       </c>
-      <c r="N15" s="145"/>
+      <c r="N15" s="141"/>
       <c r="O15" s="37">
         <v>7</v>
       </c>
       <c r="P15" s="38"/>
-      <c r="Q15" s="260">
+      <c r="Q15" s="204">
         <v>6</v>
       </c>
       <c r="R15" s="43"/>
@@ -4314,27 +4339,39 @@
         <f>SUM(C16:R16)</f>
         <v>21</v>
       </c>
-      <c r="T15" s="39"/>
+      <c r="T15" s="39">
+        <v>7</v>
+      </c>
       <c r="U15" s="40"/>
-      <c r="V15" s="37"/>
+      <c r="V15" s="37">
+        <v>6</v>
+      </c>
       <c r="W15" s="40"/>
-      <c r="X15" s="174"/>
-      <c r="Y15" s="38"/>
-      <c r="Z15" s="147"/>
-      <c r="AA15" s="43"/>
+      <c r="X15" s="170"/>
+      <c r="Y15" s="38">
+        <v>6</v>
+      </c>
+      <c r="Z15" s="143"/>
+      <c r="AA15" s="43">
+        <v>7</v>
+      </c>
       <c r="AB15" s="91">
         <f>SUM(T16:AA16)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AC15" s="41"/>
-      <c r="AD15" s="40"/>
+      <c r="AD15" s="40">
+        <v>6</v>
+      </c>
       <c r="AE15" s="42"/>
-      <c r="AF15" s="176"/>
+      <c r="AF15" s="172">
+        <v>7</v>
+      </c>
       <c r="AG15" s="91">
         <f>SUM(AC16:AF16)</f>
         <v>0</v>
       </c>
-      <c r="AH15" s="181"/>
+      <c r="AH15" s="177"/>
       <c r="AI15" s="48"/>
       <c r="AJ15" s="91">
         <f>AH16</f>
@@ -4346,7 +4383,7 @@
       </c>
       <c r="AL15" s="91">
         <f>$S15+$AB15+$AG15+$AJ15</f>
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:38" s="23" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4398,17 +4435,17 @@
       <c r="S16" s="109"/>
       <c r="T16" s="95">
         <f>(IF($T15&lt;&gt;"",($T$7*$P$40)+IF($T$7=4,($P$38)+IF($T15=$T$7+$U$7,$P$39,0),0),0)+IF($U15&lt;&gt;"",($U$7*$P$40)+IF($U$7=4,($P$38)+IF($U15=$T$7+$U$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U16" s="95"/>
       <c r="V16" s="95">
         <f>(IF($V15&lt;&gt;"",($V$7*$P$40)+IF($V$7=4,($P$38)+IF($V15=$V$7+$W$7,$P$39,0),0),0)+IF($W15&lt;&gt;"",($W$7*$P$40)+IF($W$7=4,($P$38)+IF($W15=$V$7+$W$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W16" s="95"/>
       <c r="X16" s="95">
         <f>(IF($X15&lt;&gt;"",($X$7*$P$40)+IF($X$7=4,($P$38)+IF($X15=$X$7+$Y$7,$P$39,0),0),0)+IF($Y15&lt;&gt;"",($Y$7*$P$40)+IF($Y$7=4,($P$38)+IF($Y15=$X$7+$Y$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y16" s="49"/>
       <c r="Z16" s="95">
@@ -4436,7 +4473,7 @@
       <c r="AJ16" s="90"/>
       <c r="AK16" s="67">
         <f>MAX($AL$11:$AL$33) - AL16</f>
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="AL16" s="90"/>
     </row>
@@ -4544,7 +4581,7 @@
         <f>IF(ISBLANK(T15),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="88">
         <f>IF(ISBLANK(U15),
@@ -4556,7 +4593,7 @@
         <f>IF(ISBLANK(V15),
 0,
 IF(V$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="88">
         <f>IF(ISBLANK(W15),
@@ -4574,7 +4611,7 @@
         <f>IF(ISBLANK(Y15),
 0,
 IF(Y$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z17" s="88">
         <f>IF(ISBLANK(Z15),
@@ -4629,7 +4666,7 @@
       <c r="AJ17" s="103"/>
       <c r="AK17" s="104">
         <f>SUM(C17:AI17)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AL17" s="92"/>
     </row>
@@ -4827,82 +4864,94 @@
       <c r="AL18" s="92"/>
     </row>
     <row r="19" spans="1:38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="148">
+      <c r="A19" s="144">
         <f>RANK(AL19,$AL$11:$AL$33,)</f>
         <v>5</v>
       </c>
-      <c r="B19" s="149" t="s">
+      <c r="B19" s="145" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="161">
+      <c r="C19" s="157">
         <v>6</v>
       </c>
-      <c r="D19" s="162"/>
-      <c r="E19" s="177"/>
-      <c r="F19" s="162">
+      <c r="D19" s="158"/>
+      <c r="E19" s="173"/>
+      <c r="F19" s="158">
         <v>7</v>
       </c>
-      <c r="G19" s="178">
+      <c r="G19" s="174">
         <v>4</v>
       </c>
-      <c r="H19" s="164"/>
-      <c r="I19" s="177"/>
-      <c r="J19" s="164">
+      <c r="H19" s="160"/>
+      <c r="I19" s="173"/>
+      <c r="J19" s="160">
         <v>6</v>
       </c>
-      <c r="K19" s="166">
+      <c r="K19" s="162">
         <v>5</v>
       </c>
-      <c r="L19" s="164"/>
-      <c r="M19" s="165">
+      <c r="L19" s="160"/>
+      <c r="M19" s="161">
         <v>7</v>
       </c>
-      <c r="N19" s="162"/>
-      <c r="O19" s="165">
+      <c r="N19" s="158"/>
+      <c r="O19" s="161">
         <v>7</v>
       </c>
-      <c r="P19" s="162"/>
-      <c r="Q19" s="163"/>
-      <c r="R19" s="168">
+      <c r="P19" s="158"/>
+      <c r="Q19" s="159"/>
+      <c r="R19" s="164">
         <v>7</v>
       </c>
-      <c r="S19" s="169">
+      <c r="S19" s="165">
         <f>SUM(C20:R20)</f>
         <v>9</v>
       </c>
-      <c r="T19" s="161"/>
-      <c r="U19" s="164"/>
-      <c r="V19" s="165"/>
-      <c r="W19" s="164"/>
-      <c r="X19" s="175"/>
-      <c r="Y19" s="162"/>
-      <c r="Z19" s="163"/>
-      <c r="AA19" s="168"/>
-      <c r="AB19" s="170">
+      <c r="T19" s="157"/>
+      <c r="U19" s="160">
+        <v>5</v>
+      </c>
+      <c r="V19" s="161"/>
+      <c r="W19" s="160">
+        <v>7</v>
+      </c>
+      <c r="X19" s="171"/>
+      <c r="Y19" s="158">
+        <v>5</v>
+      </c>
+      <c r="Z19" s="159"/>
+      <c r="AA19" s="164">
+        <v>5</v>
+      </c>
+      <c r="AB19" s="166">
         <f>SUM(T20:AA20)</f>
-        <v>0</v>
-      </c>
-      <c r="AC19" s="163"/>
-      <c r="AD19" s="164"/>
-      <c r="AE19" s="166"/>
-      <c r="AF19" s="173"/>
-      <c r="AG19" s="170">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="159"/>
+      <c r="AD19" s="160">
+        <v>6</v>
+      </c>
+      <c r="AE19" s="162"/>
+      <c r="AF19" s="169">
+        <v>6</v>
+      </c>
+      <c r="AG19" s="166">
         <f>SUM(AC20:AF20)</f>
         <v>0</v>
       </c>
-      <c r="AH19" s="180"/>
-      <c r="AI19" s="171"/>
-      <c r="AJ19" s="170">
+      <c r="AH19" s="176"/>
+      <c r="AI19" s="167"/>
+      <c r="AJ19" s="166">
         <f>AH20</f>
         <v>0</v>
       </c>
-      <c r="AK19" s="172">
+      <c r="AK19" s="168">
         <f>MAX($AL$11:$AL$33) - AL19</f>
-        <v>17</v>
-      </c>
-      <c r="AL19" s="170">
+        <v>23</v>
+      </c>
+      <c r="AL19" s="166">
         <f>$S19+$AB19+$AG19+$AJ19</f>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:38" s="23" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4964,7 +5013,7 @@
       <c r="W20" s="95"/>
       <c r="X20" s="95">
         <f>(IF($X19&lt;&gt;"",($X$7*$P$40)+IF($X$7=4,($P$38)+IF($X19=$X$7+$Y$7,$P$39,0),0),0)+IF($Y19&lt;&gt;"",($Y$7*$P$40)+IF($Y$7=4,($P$38)+IF($Y19=$X$7+$Y$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y20" s="49"/>
       <c r="Z20" s="95">
@@ -4992,7 +5041,7 @@
       <c r="AJ20" s="109"/>
       <c r="AK20" s="36">
         <f>MAX($AL$11:$AL$33) - AL20</f>
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="AL20" s="90"/>
     </row>
@@ -5130,7 +5179,7 @@
         <f>IF(ISBLANK(Y19),
 0,
 IF(Y$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21" s="88">
         <f>IF(ISBLANK(Z19),
@@ -5185,7 +5234,7 @@
       <c r="AJ21" s="103"/>
       <c r="AK21" s="104">
         <f>SUM(C21:AI21)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL21" s="92"/>
     </row>
@@ -5402,7 +5451,7 @@
       <c r="H23" s="40">
         <v>6</v>
       </c>
-      <c r="I23" s="253">
+      <c r="I23" s="197">
         <v>7</v>
       </c>
       <c r="J23" s="40"/>
@@ -5414,7 +5463,7 @@
       <c r="N23" s="38">
         <v>5</v>
       </c>
-      <c r="O23" s="253">
+      <c r="O23" s="197">
         <v>5</v>
       </c>
       <c r="P23" s="38"/>
@@ -5427,26 +5476,38 @@
         <v>13</v>
       </c>
       <c r="T23" s="39"/>
-      <c r="U23" s="40"/>
+      <c r="U23" s="40">
+        <v>6</v>
+      </c>
       <c r="V23" s="37"/>
-      <c r="W23" s="40"/>
+      <c r="W23" s="40">
+        <v>6</v>
+      </c>
       <c r="X23" s="42"/>
-      <c r="Y23" s="38"/>
+      <c r="Y23" s="38">
+        <v>6</v>
+      </c>
       <c r="Z23" s="41"/>
-      <c r="AA23" s="43"/>
+      <c r="AA23" s="43">
+        <v>7</v>
+      </c>
       <c r="AB23" s="91">
         <f>SUM(T24:AA24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC23" s="41"/>
-      <c r="AD23" s="40"/>
-      <c r="AE23" s="42"/>
+      <c r="AD23" s="40">
+        <v>6</v>
+      </c>
+      <c r="AE23" s="42">
+        <v>5</v>
+      </c>
       <c r="AF23" s="40"/>
       <c r="AG23" s="91">
         <f>SUM(AC24:AF24)</f>
         <v>0</v>
       </c>
-      <c r="AH23" s="179"/>
+      <c r="AH23" s="175"/>
       <c r="AI23" s="47"/>
       <c r="AJ23" s="91">
         <f>AH24</f>
@@ -5454,11 +5515,11 @@
       </c>
       <c r="AK23" s="82">
         <f>MAX($AL$11:$AL$33) - AL23</f>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="AL23" s="91">
         <f>$S23+$AB23+$AG23+$AJ23</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:38" s="23" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5520,7 +5581,7 @@
       <c r="W24" s="95"/>
       <c r="X24" s="95">
         <f>(IF($X23&lt;&gt;"",($X$7*$P$40)+IF($X$7=4,($P$38)+IF($X23=$X$7+$Y$7,$P$39,0),0),0)+IF($Y23&lt;&gt;"",($Y$7*$P$40)+IF($Y$7=4,($P$38)+IF($Y23=$X$7+$Y$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y24" s="49"/>
       <c r="Z24" s="102">
@@ -5548,7 +5609,7 @@
       <c r="AJ24" s="109"/>
       <c r="AK24" s="36">
         <f>MAX($AL$11:$AL$33) - AL24</f>
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="AL24" s="90"/>
     </row>
@@ -5686,7 +5747,7 @@
         <f>IF(ISBLANK(Y23),
 0,
 IF(Y$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z25" s="102">
         <f>IF(ISBLANK(Z23),
@@ -5741,7 +5802,7 @@
       <c r="AJ25" s="103"/>
       <c r="AK25" s="104">
         <f>SUM(C25:AI25)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL25" s="92"/>
     </row>
@@ -5939,82 +6000,94 @@
       <c r="AL26" s="92"/>
     </row>
     <row r="27" spans="1:38" s="23" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="148">
+      <c r="A27" s="144">
         <f>RANK(AL27,$AL$11:$AL$33,)</f>
         <v>3</v>
       </c>
-      <c r="B27" s="149" t="s">
+      <c r="B27" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="161">
+      <c r="C27" s="157">
         <v>5</v>
       </c>
-      <c r="D27" s="162"/>
-      <c r="E27" s="165">
+      <c r="D27" s="158"/>
+      <c r="E27" s="161">
         <v>7</v>
       </c>
-      <c r="F27" s="162"/>
-      <c r="G27" s="188">
+      <c r="F27" s="158"/>
+      <c r="G27" s="184">
         <v>6</v>
       </c>
-      <c r="H27" s="164"/>
-      <c r="I27" s="165"/>
-      <c r="J27" s="164">
+      <c r="H27" s="160"/>
+      <c r="I27" s="161"/>
+      <c r="J27" s="160">
         <v>6</v>
       </c>
-      <c r="K27" s="166">
+      <c r="K27" s="162">
         <v>5</v>
       </c>
-      <c r="L27" s="164"/>
-      <c r="M27" s="165">
+      <c r="L27" s="160"/>
+      <c r="M27" s="161">
         <v>7</v>
       </c>
-      <c r="N27" s="167"/>
-      <c r="O27" s="165">
+      <c r="N27" s="163"/>
+      <c r="O27" s="161">
         <v>6</v>
       </c>
-      <c r="P27" s="162"/>
-      <c r="Q27" s="163">
+      <c r="P27" s="158"/>
+      <c r="Q27" s="159">
         <v>7</v>
       </c>
-      <c r="R27" s="168"/>
-      <c r="S27" s="170">
+      <c r="R27" s="164"/>
+      <c r="S27" s="166">
         <f>SUM(C28:R28)</f>
         <v>17</v>
       </c>
-      <c r="T27" s="161"/>
-      <c r="U27" s="164"/>
-      <c r="V27" s="165"/>
-      <c r="W27" s="164"/>
-      <c r="X27" s="166"/>
-      <c r="Y27" s="162"/>
-      <c r="Z27" s="163"/>
-      <c r="AA27" s="168"/>
-      <c r="AB27" s="170">
+      <c r="T27" s="157">
+        <v>7</v>
+      </c>
+      <c r="U27" s="160"/>
+      <c r="V27" s="161"/>
+      <c r="W27" s="160">
+        <v>7</v>
+      </c>
+      <c r="X27" s="162"/>
+      <c r="Y27" s="158">
+        <v>7</v>
+      </c>
+      <c r="Z27" s="159"/>
+      <c r="AA27" s="164">
+        <v>7</v>
+      </c>
+      <c r="AB27" s="166">
         <f>SUM(T28:AA28)</f>
-        <v>0</v>
-      </c>
-      <c r="AC27" s="163"/>
-      <c r="AD27" s="164"/>
-      <c r="AE27" s="166"/>
-      <c r="AF27" s="173"/>
-      <c r="AG27" s="170">
+        <v>8</v>
+      </c>
+      <c r="AC27" s="159">
+        <v>6</v>
+      </c>
+      <c r="AD27" s="160"/>
+      <c r="AE27" s="162"/>
+      <c r="AF27" s="169">
+        <v>7</v>
+      </c>
+      <c r="AG27" s="166">
         <f>SUM(AC28:AF28)</f>
         <v>0</v>
       </c>
-      <c r="AH27" s="158"/>
-      <c r="AI27" s="159"/>
-      <c r="AJ27" s="170">
+      <c r="AH27" s="154"/>
+      <c r="AI27" s="155"/>
+      <c r="AJ27" s="166">
         <f>AH28</f>
         <v>0</v>
       </c>
-      <c r="AK27" s="172">
+      <c r="AK27" s="168">
         <f>MAX($AL$11:$AL$33) - AL27</f>
-        <v>9</v>
-      </c>
-      <c r="AL27" s="187">
+        <v>10</v>
+      </c>
+      <c r="AL27" s="183">
         <f>$S27+$AB27+$AG27+$AJ27</f>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:38" s="23" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6066,7 +6139,7 @@
       <c r="S28" s="109"/>
       <c r="T28" s="95">
         <f>(IF($T27&lt;&gt;"",($T$7*$P$40)+IF($T$7=4,($P$38)+IF($T27=$T$7+$U$7,$P$39,0),0),0)+IF($U27&lt;&gt;"",($U$7*$P$40)+IF($U$7=4,($P$38)+IF($U27=$T$7+$U$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U28" s="95"/>
       <c r="V28" s="95">
@@ -6076,7 +6149,7 @@
       <c r="W28" s="95"/>
       <c r="X28" s="95">
         <f>(IF($X27&lt;&gt;"",($X$7*$P$40)+IF($X$7=4,($P$38)+IF($X27=$X$7+$Y$7,$P$39,0),0),0)+IF($Y27&lt;&gt;"",($Y$7*$P$40)+IF($Y$7=4,($P$38)+IF($Y27=$X$7+$Y$7,$P$39,0),0),0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y28" s="49"/>
       <c r="Z28" s="102">
@@ -6104,7 +6177,7 @@
       <c r="AJ28" s="109"/>
       <c r="AK28" s="36">
         <f>MAX($AL$11:$AL$33) - AL28</f>
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="AL28" s="90"/>
     </row>
@@ -6212,7 +6285,7 @@
         <f>IF(ISBLANK(T27),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29" s="88">
         <f>IF(ISBLANK(U27),
@@ -6242,7 +6315,7 @@
         <f>IF(ISBLANK(Y27),
 0,
 IF(Y$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z29" s="102">
         <f>IF(ISBLANK(Z27),
@@ -6297,7 +6370,7 @@
       <c r="AJ29" s="103"/>
       <c r="AK29" s="104">
         <f>SUM(C29:AI29)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AL29" s="92"/>
     </row>
@@ -6435,7 +6508,7 @@
         <f>IF(Y29 = 0,
 0,
 IF(Y27 = (X$7+Y$7),1,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z30" s="102">
         <f>IF(Z29 = 0,
@@ -6490,7 +6563,7 @@
       <c r="AJ30" s="103"/>
       <c r="AK30" s="104">
         <f>SUM(C30:AI30)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL30" s="92"/>
     </row>
@@ -6687,7 +6760,7 @@
         <f>IF(ISBLANK(#REF!),
 0,
 IF(T$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32" s="88">
         <f>IF(ISBLANK(#REF!),
@@ -6699,7 +6772,7 @@
         <f>IF(ISBLANK(#REF!),
 0,
 IF(V$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W32" s="88">
         <f>IF(ISBLANK(#REF!),
@@ -6717,13 +6790,13 @@
         <f>IF(ISBLANK(#REF!),
 0,
 IF(Y$7 = 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z32" s="88">
         <f>IF(ISBLANK(#REF!),
 0,
 IF(Z$7= 4, 1, 0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA32" s="88">
         <f>IF(ISBLANK(#REF!),
@@ -6772,7 +6845,7 @@
       <c r="AJ32" s="103"/>
       <c r="AK32" s="104">
         <f>SUM(C32:AI32)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="AL32" s="92"/>
     </row>
@@ -6878,11 +6951,11 @@
         <v>0</v>
       </c>
       <c r="S33" s="103"/>
-      <c r="T33" s="88">
+      <c r="T33" s="88" t="e">
         <f>IF(T32 = 0,
 0,
 IF(#REF! = (T$7+U$7),1,0))</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="U33" s="88">
         <f>IF(U32 = 0,
@@ -6890,11 +6963,11 @@
 IF(#REF! = (T$7+U$7),1,0))</f>
         <v>0</v>
       </c>
-      <c r="V33" s="88">
+      <c r="V33" s="88" t="e">
         <f>IF(V32 = 0,
 0,
 IF(#REF! = (V$7+W$7),1,0))</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="W33" s="88">
         <f>IF(W32 = 0,
@@ -6908,17 +6981,17 @@
 IF(#REF! = (X$7+Y$7),1,0))</f>
         <v>0</v>
       </c>
-      <c r="Y33" s="88">
+      <c r="Y33" s="88" t="e">
         <f>IF(Y32 = 0,
 0,
 IF(#REF! = (X$7+Y$7),1,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Z33" s="88">
+        <v>#REF!</v>
+      </c>
+      <c r="Z33" s="88" t="e">
         <f>IF(Z32 = 0,
 0,
 IF(#REF! = (Z$7+AA$7),1,0))</f>
-        <v>0</v>
+        <v>#REF!</v>
       </c>
       <c r="AA33" s="88">
         <f>IF(AA32 = 0,
@@ -6969,124 +7042,124 @@
         <f>SUM(C33:AI33)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL33" s="137"/>
+      <c r="AL33" s="133"/>
     </row>
     <row r="34" spans="1:38" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="51"/>
       <c r="B34" s="45"/>
-      <c r="C34" s="140">
+      <c r="C34" s="136">
         <f xml:space="preserve"> COUNT(C11,C15,C19,C23,C27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>4</v>
       </c>
-      <c r="D34" s="138">
+      <c r="D34" s="134">
         <f xml:space="preserve"> COUNT(D11,D15,D19,D23,D27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>1</v>
       </c>
-      <c r="E34" s="140">
+      <c r="E34" s="136">
         <f xml:space="preserve"> COUNT(E11,E15,E19,E23,E27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>3</v>
       </c>
-      <c r="F34" s="138">
+      <c r="F34" s="134">
         <f xml:space="preserve"> COUNT(F11,F15,F19,F23,F27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>2</v>
       </c>
-      <c r="G34" s="140">
+      <c r="G34" s="136">
         <f xml:space="preserve"> COUNT(G11,G15,G19,G23,G27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>4</v>
       </c>
-      <c r="H34" s="138">
+      <c r="H34" s="134">
         <f xml:space="preserve"> COUNT(H11,H15,H19,H23,H27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>1</v>
       </c>
-      <c r="I34" s="140">
+      <c r="I34" s="136">
         <f xml:space="preserve"> COUNT(I11,I15,I19,I23,I27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>1</v>
       </c>
-      <c r="J34" s="146">
+      <c r="J34" s="142">
         <f xml:space="preserve"> COUNT(J11,J15,J19,J23,J27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>4</v>
       </c>
-      <c r="K34" s="139">
+      <c r="K34" s="135">
         <f xml:space="preserve"> COUNT(K11,K15,K19,K23,K27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>4</v>
       </c>
-      <c r="L34" s="138">
+      <c r="L34" s="134">
         <f xml:space="preserve"> COUNT(L11,L15,L19,L23,L27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>1</v>
       </c>
-      <c r="M34" s="140">
+      <c r="M34" s="136">
         <f xml:space="preserve"> COUNT(M11,M15,M19,M23,M27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>4</v>
       </c>
-      <c r="N34" s="138">
+      <c r="N34" s="134">
         <f xml:space="preserve"> COUNT(N11,N15,N19,N23,N27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>1</v>
       </c>
-      <c r="O34" s="140">
+      <c r="O34" s="136">
         <f xml:space="preserve"> COUNT(O11,O15,O19,O23,O27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>5</v>
       </c>
-      <c r="P34" s="138">
+      <c r="P34" s="134">
         <f xml:space="preserve"> COUNT(P11,P15,P19,P23,P27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>0</v>
       </c>
-      <c r="Q34" s="140">
+      <c r="Q34" s="136">
         <f xml:space="preserve"> COUNT(Q11,Q15,Q19,Q23,Q27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>3</v>
       </c>
-      <c r="R34" s="141">
+      <c r="R34" s="137">
         <f xml:space="preserve"> COUNT(R11,R15,R19,R23,R27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>2</v>
       </c>
       <c r="S34" s="56"/>
-      <c r="T34" s="140">
+      <c r="T34" s="136">
         <f xml:space="preserve"> COUNT(T11,T15,T19,T23,T27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="U34" s="138">
+        <v>2</v>
+      </c>
+      <c r="U34" s="134">
         <f xml:space="preserve"> COUNT(U11,U15,U19,U23,U27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="V34" s="140">
+        <v>3</v>
+      </c>
+      <c r="V34" s="136">
         <f xml:space="preserve"> COUNT(V11,V15,V19,V23,V27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="W34" s="146">
+        <v>2</v>
+      </c>
+      <c r="W34" s="142">
         <f xml:space="preserve"> COUNT(W11,W15,W19,W23,W27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="X34" s="139">
+        <v>3</v>
+      </c>
+      <c r="X34" s="135">
         <f xml:space="preserve"> COUNT(X11,X15,X19,X23,X27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
         <v>0</v>
       </c>
-      <c r="Y34" s="138">
+      <c r="Y34" s="134">
         <f xml:space="preserve"> COUNT(Y11,Y15,Y19,Y23,Y27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="Z34" s="140">
+        <v>5</v>
+      </c>
+      <c r="Z34" s="136">
         <f xml:space="preserve"> COUNT(Z11,Z15,Z19,Z23,Z27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
-      </c>
-      <c r="AA34" s="141">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="137">
         <f xml:space="preserve"> COUNT(AA11,AA15,AA19,AA23,AA27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB34" s="75"/>
       <c r="AC34" s="52">
         <f xml:space="preserve"> COUNT(AC11,AC15,AC19,AC23,AC27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD34" s="53">
         <f xml:space="preserve"> COUNT(AD11,AD15,AD19,AD23,AD27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AE34" s="54">
         <f xml:space="preserve"> COUNT(AE11,AE15,AE19,AE23,AE27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF34" s="55">
         <f xml:space="preserve"> COUNT(AF11,AF15,AF19,AF23,AF27,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!,#REF!)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AG34" s="75"/>
       <c r="AH34" s="57">
@@ -7104,12 +7177,12 @@
     <row r="36" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
       <c r="N36" s="22"/>
-      <c r="O36" s="238" t="s">
+      <c r="O36" s="246" t="s">
         <v>17</v>
       </c>
-      <c r="P36" s="239"/>
-      <c r="Q36" s="239"/>
-      <c r="R36" s="240"/>
+      <c r="P36" s="247"/>
+      <c r="Q36" s="247"/>
+      <c r="R36" s="248"/>
       <c r="AG36" s="25"/>
       <c r="AH36" s="25"/>
       <c r="AI36" s="25"/>
@@ -7118,21 +7191,21 @@
     </row>
     <row r="37" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
-      <c r="B37" s="228" t="s">
+      <c r="B37" s="236" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="229"/>
-      <c r="D37" s="229"/>
-      <c r="E37" s="229"/>
-      <c r="F37" s="229"/>
-      <c r="G37" s="229"/>
-      <c r="H37" s="229"/>
-      <c r="I37" s="229"/>
-      <c r="J37" s="229"/>
-      <c r="K37" s="229"/>
-      <c r="L37" s="229"/>
-      <c r="M37" s="229"/>
-      <c r="N37" s="230"/>
+      <c r="C37" s="237"/>
+      <c r="D37" s="237"/>
+      <c r="E37" s="237"/>
+      <c r="F37" s="237"/>
+      <c r="G37" s="237"/>
+      <c r="H37" s="237"/>
+      <c r="I37" s="237"/>
+      <c r="J37" s="237"/>
+      <c r="K37" s="237"/>
+      <c r="L37" s="237"/>
+      <c r="M37" s="237"/>
+      <c r="N37" s="238"/>
       <c r="O37" s="17">
         <v>1</v>
       </c>
@@ -7145,43 +7218,43 @@
       <c r="R37" s="18">
         <v>4</v>
       </c>
-      <c r="U37" s="241" t="s">
+      <c r="U37" s="249" t="s">
         <v>26</v>
       </c>
-      <c r="V37" s="242"/>
-      <c r="W37" s="242"/>
-      <c r="X37" s="242"/>
-      <c r="Y37" s="242"/>
-      <c r="Z37" s="242"/>
-      <c r="AA37" s="242"/>
-      <c r="AB37" s="242"/>
-      <c r="AC37" s="242"/>
-      <c r="AD37" s="243"/>
-      <c r="AG37" s="244" t="s">
+      <c r="V37" s="250"/>
+      <c r="W37" s="250"/>
+      <c r="X37" s="250"/>
+      <c r="Y37" s="250"/>
+      <c r="Z37" s="250"/>
+      <c r="AA37" s="250"/>
+      <c r="AB37" s="250"/>
+      <c r="AC37" s="250"/>
+      <c r="AD37" s="251"/>
+      <c r="AG37" s="252" t="s">
         <v>24</v>
       </c>
-      <c r="AH37" s="245"/>
-      <c r="AI37" s="245"/>
-      <c r="AJ37" s="245"/>
-      <c r="AK37" s="246"/>
+      <c r="AH37" s="253"/>
+      <c r="AI37" s="253"/>
+      <c r="AJ37" s="253"/>
+      <c r="AK37" s="254"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
-      <c r="B38" s="218" t="s">
+      <c r="B38" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="219"/>
-      <c r="D38" s="219"/>
-      <c r="E38" s="219"/>
-      <c r="F38" s="219"/>
-      <c r="G38" s="219"/>
-      <c r="H38" s="219"/>
-      <c r="I38" s="219"/>
-      <c r="J38" s="219"/>
-      <c r="K38" s="219"/>
-      <c r="L38" s="219"/>
-      <c r="M38" s="219"/>
-      <c r="N38" s="220"/>
+      <c r="C38" s="217"/>
+      <c r="D38" s="217"/>
+      <c r="E38" s="217"/>
+      <c r="F38" s="217"/>
+      <c r="G38" s="217"/>
+      <c r="H38" s="217"/>
+      <c r="I38" s="217"/>
+      <c r="J38" s="217"/>
+      <c r="K38" s="217"/>
+      <c r="L38" s="217"/>
+      <c r="M38" s="217"/>
+      <c r="N38" s="218"/>
       <c r="O38" s="16">
         <v>3</v>
       </c>
@@ -7194,49 +7267,49 @@
       <c r="R38" s="19">
         <v>3</v>
       </c>
-      <c r="U38" s="233" t="s">
+      <c r="U38" s="241" t="s">
         <v>20</v>
       </c>
-      <c r="V38" s="234"/>
-      <c r="W38" s="234"/>
-      <c r="X38" s="234"/>
-      <c r="Y38" s="234"/>
-      <c r="Z38" s="234"/>
-      <c r="AA38" s="234"/>
-      <c r="AB38" s="231">
+      <c r="V38" s="242"/>
+      <c r="W38" s="242"/>
+      <c r="X38" s="242"/>
+      <c r="Y38" s="242"/>
+      <c r="Z38" s="242"/>
+      <c r="AA38" s="242"/>
+      <c r="AB38" s="239">
         <v>5</v>
       </c>
-      <c r="AC38" s="231"/>
-      <c r="AD38" s="232"/>
+      <c r="AC38" s="239"/>
+      <c r="AD38" s="240"/>
       <c r="AE38" s="24"/>
       <c r="AF38" s="24"/>
-      <c r="AG38" s="247" t="s">
+      <c r="AG38" s="213" t="s">
         <v>21</v>
       </c>
-      <c r="AH38" s="248"/>
-      <c r="AI38" s="248"/>
-      <c r="AJ38" s="249"/>
-      <c r="AK38" s="142">
+      <c r="AH38" s="214"/>
+      <c r="AI38" s="214"/>
+      <c r="AJ38" s="215"/>
+      <c r="AK38" s="138">
         <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
-      <c r="B39" s="218" t="s">
+      <c r="B39" s="223" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="219"/>
-      <c r="D39" s="219"/>
-      <c r="E39" s="219"/>
-      <c r="F39" s="219"/>
-      <c r="G39" s="219"/>
-      <c r="H39" s="219"/>
-      <c r="I39" s="219"/>
-      <c r="J39" s="219"/>
-      <c r="K39" s="219"/>
-      <c r="L39" s="219"/>
-      <c r="M39" s="219"/>
-      <c r="N39" s="220"/>
+      <c r="C39" s="217"/>
+      <c r="D39" s="217"/>
+      <c r="E39" s="217"/>
+      <c r="F39" s="217"/>
+      <c r="G39" s="217"/>
+      <c r="H39" s="217"/>
+      <c r="I39" s="217"/>
+      <c r="J39" s="217"/>
+      <c r="K39" s="217"/>
+      <c r="L39" s="217"/>
+      <c r="M39" s="217"/>
+      <c r="N39" s="218"/>
       <c r="O39" s="16">
         <v>2</v>
       </c>
@@ -7249,49 +7322,49 @@
       <c r="R39" s="19">
         <v>2</v>
       </c>
-      <c r="U39" s="223" t="s">
+      <c r="U39" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="V39" s="224"/>
-      <c r="W39" s="224"/>
-      <c r="X39" s="224"/>
-      <c r="Y39" s="224"/>
-      <c r="Z39" s="224"/>
-      <c r="AA39" s="224"/>
-      <c r="AB39" s="251">
+      <c r="V39" s="220"/>
+      <c r="W39" s="220"/>
+      <c r="X39" s="220"/>
+      <c r="Y39" s="220"/>
+      <c r="Z39" s="220"/>
+      <c r="AA39" s="220"/>
+      <c r="AB39" s="221">
         <v>20</v>
       </c>
-      <c r="AC39" s="251"/>
-      <c r="AD39" s="252"/>
+      <c r="AC39" s="221"/>
+      <c r="AD39" s="222"/>
       <c r="AE39" s="24"/>
       <c r="AF39" s="24"/>
-      <c r="AG39" s="250" t="s">
+      <c r="AG39" s="216" t="s">
         <v>22</v>
       </c>
-      <c r="AH39" s="219"/>
-      <c r="AI39" s="219"/>
-      <c r="AJ39" s="220"/>
+      <c r="AH39" s="217"/>
+      <c r="AI39" s="217"/>
+      <c r="AJ39" s="218"/>
       <c r="AK39" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29"/>
-      <c r="B40" s="225" t="s">
+      <c r="B40" s="233" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="226"/>
-      <c r="D40" s="226"/>
-      <c r="E40" s="226"/>
-      <c r="F40" s="226"/>
-      <c r="G40" s="226"/>
-      <c r="H40" s="226"/>
-      <c r="I40" s="226"/>
-      <c r="J40" s="226"/>
-      <c r="K40" s="226"/>
-      <c r="L40" s="226"/>
-      <c r="M40" s="226"/>
-      <c r="N40" s="227"/>
+      <c r="C40" s="234"/>
+      <c r="D40" s="234"/>
+      <c r="E40" s="234"/>
+      <c r="F40" s="234"/>
+      <c r="G40" s="234"/>
+      <c r="H40" s="234"/>
+      <c r="I40" s="234"/>
+      <c r="J40" s="234"/>
+      <c r="K40" s="234"/>
+      <c r="L40" s="234"/>
+      <c r="M40" s="234"/>
+      <c r="N40" s="235"/>
       <c r="O40" s="3">
         <v>0</v>
       </c>
@@ -7304,52 +7377,52 @@
       <c r="R40" s="20">
         <v>0</v>
       </c>
-      <c r="U40" s="235" t="s">
+      <c r="U40" s="243" t="s">
         <v>19</v>
       </c>
-      <c r="V40" s="222"/>
-      <c r="W40" s="222"/>
-      <c r="X40" s="222"/>
-      <c r="Y40" s="222"/>
-      <c r="Z40" s="222"/>
-      <c r="AA40" s="222"/>
-      <c r="AB40" s="236">
+      <c r="V40" s="225"/>
+      <c r="W40" s="225"/>
+      <c r="X40" s="225"/>
+      <c r="Y40" s="225"/>
+      <c r="Z40" s="225"/>
+      <c r="AA40" s="225"/>
+      <c r="AB40" s="244">
         <f>AB38*AB39</f>
         <v>100</v>
       </c>
-      <c r="AC40" s="236"/>
-      <c r="AD40" s="237"/>
+      <c r="AC40" s="244"/>
+      <c r="AD40" s="245"/>
       <c r="AE40" s="24"/>
       <c r="AF40" s="24"/>
-      <c r="AG40" s="250" t="s">
+      <c r="AG40" s="216" t="s">
         <v>25</v>
       </c>
-      <c r="AH40" s="219"/>
-      <c r="AI40" s="219"/>
-      <c r="AJ40" s="220"/>
+      <c r="AH40" s="217"/>
+      <c r="AI40" s="217"/>
+      <c r="AJ40" s="218"/>
       <c r="AK40" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG41" s="223" t="s">
+      <c r="AG41" s="219" t="s">
         <v>23</v>
       </c>
-      <c r="AH41" s="224"/>
-      <c r="AI41" s="224"/>
-      <c r="AJ41" s="224"/>
-      <c r="AK41" s="144">
+      <c r="AH41" s="220"/>
+      <c r="AI41" s="220"/>
+      <c r="AJ41" s="220"/>
+      <c r="AK41" s="140">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:38" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AG42" s="221" t="s">
+      <c r="AG42" s="224" t="s">
         <v>19</v>
       </c>
-      <c r="AH42" s="222"/>
-      <c r="AI42" s="222"/>
-      <c r="AJ42" s="222"/>
-      <c r="AK42" s="143">
+      <c r="AH42" s="225"/>
+      <c r="AI42" s="225"/>
+      <c r="AJ42" s="225"/>
+      <c r="AK42" s="139">
         <f>SUM(AK38:AK41)</f>
         <v>100</v>
       </c>
@@ -7360,11 +7433,25 @@
     <sortCondition ref="B11:B30"/>
   </sortState>
   <mergeCells count="40">
-    <mergeCell ref="AG38:AJ38"/>
-    <mergeCell ref="AG40:AJ40"/>
-    <mergeCell ref="AG39:AJ39"/>
-    <mergeCell ref="U39:AA39"/>
-    <mergeCell ref="AB39:AD39"/>
+    <mergeCell ref="C5:S5"/>
+    <mergeCell ref="T5:AB5"/>
+    <mergeCell ref="AC5:AG5"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="AH5:AJ5"/>
+    <mergeCell ref="AG6:AG10"/>
+    <mergeCell ref="AJ6:AJ10"/>
+    <mergeCell ref="X6:AA6"/>
+    <mergeCell ref="AB6:AB10"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="P1:AJ1"/>
+    <mergeCell ref="C4:O4"/>
+    <mergeCell ref="P4:AJ4"/>
+    <mergeCell ref="C3:P3"/>
+    <mergeCell ref="Q3:AJ3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="Q2:AJ2"/>
     <mergeCell ref="B39:N39"/>
     <mergeCell ref="AG42:AJ42"/>
     <mergeCell ref="AG41:AJ41"/>
@@ -7381,25 +7468,11 @@
     <mergeCell ref="O36:R36"/>
     <mergeCell ref="U37:AD37"/>
     <mergeCell ref="AG37:AK37"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="P1:AJ1"/>
-    <mergeCell ref="C4:O4"/>
-    <mergeCell ref="P4:AJ4"/>
-    <mergeCell ref="C3:P3"/>
-    <mergeCell ref="Q3:AJ3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="Q2:AJ2"/>
-    <mergeCell ref="C5:S5"/>
-    <mergeCell ref="T5:AB5"/>
-    <mergeCell ref="AC5:AG5"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="AH5:AJ5"/>
-    <mergeCell ref="AG6:AG10"/>
-    <mergeCell ref="AJ6:AJ10"/>
-    <mergeCell ref="X6:AA6"/>
-    <mergeCell ref="AB6:AB10"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG38:AJ38"/>
+    <mergeCell ref="AG40:AJ40"/>
+    <mergeCell ref="AG39:AJ39"/>
+    <mergeCell ref="U39:AA39"/>
+    <mergeCell ref="AB39:AD39"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="C34:D34">
@@ -7632,7 +7705,7 @@
     <hyperlink ref="Q2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.39370078740157483"/>
-  <pageSetup paperSize="5" scale="99" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="5" scale="86" orientation="landscape" r:id="rId3"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;20Pool des séries - Sauf une fois au chalet&amp;R
 Dernière mise à jour: &amp;D - &amp;T</oddHeader>
@@ -7816,8 +7889,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8035,21 +8108,31 @@
       <c r="K6" s="15"/>
       <c r="L6" s="12"/>
       <c r="M6" s="60" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="N6" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
+        <v>54</v>
+      </c>
+      <c r="O6" s="62">
+        <v>4</v>
+      </c>
+      <c r="P6" s="62">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="62">
+        <v>3</v>
+      </c>
+      <c r="R6" s="62">
+        <v>1</v>
+      </c>
+      <c r="S6" s="62">
+        <v>3</v>
+      </c>
       <c r="T6" s="62"/>
       <c r="U6" s="62"/>
       <c r="V6" s="61">
         <f>IF(O6&gt;O7,1,0)+IF(P6&gt;P7,1,0)+IF(Q6&gt;Q7,1,0)+IF(R6&gt;R7,1,0)+IF(S6&gt;S7,1,0)+IF(T6&gt;T7,1,0)+IF(U6&gt;U7,1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W6" s="12"/>
       <c r="Y6" s="67"/>
@@ -8094,21 +8177,31 @@
       </c>
       <c r="K7" s="45"/>
       <c r="M7" s="60" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="N7" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
+        <v>41</v>
+      </c>
+      <c r="O7" s="62">
+        <v>2</v>
+      </c>
+      <c r="P7" s="62">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="62">
+        <v>2</v>
+      </c>
+      <c r="R7" s="62">
+        <v>2</v>
+      </c>
+      <c r="S7" s="62">
+        <v>2</v>
+      </c>
       <c r="T7" s="62"/>
       <c r="U7" s="62"/>
       <c r="V7" s="61">
         <f>IF(O7&gt;O6,1,0)+IF(P7&gt;P6,1,0)+IF(Q7&gt;Q6,1,0)+IF(R7&gt;R6,1,0)+IF(S7&gt;S6,1,0)+IF(T7&gt;T6,1,0)+IF(U7&gt;U6,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="13"/>
       <c r="Y7" s="67"/>
@@ -8144,9 +8237,11 @@
       <c r="W8" s="13"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z8" s="64"/>
+        <v>49</v>
+      </c>
+      <c r="Z8" s="64" t="s">
+        <v>54</v>
+      </c>
       <c r="AA8" s="62"/>
       <c r="AB8" s="62"/>
       <c r="AC8" s="62"/>
@@ -8183,9 +8278,11 @@
       <c r="V9" s="2"/>
       <c r="W9" s="13"/>
       <c r="Y9" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z9" s="64"/>
+        <v>30</v>
+      </c>
+      <c r="Z9" s="64" t="s">
+        <v>55</v>
+      </c>
       <c r="AA9" s="62"/>
       <c r="AB9" s="62"/>
       <c r="AC9" s="62"/>
@@ -8237,16 +8334,26 @@
       <c r="N10" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
+      <c r="O10" s="62">
+        <v>5</v>
+      </c>
+      <c r="P10" s="62">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="62">
+        <v>4</v>
+      </c>
+      <c r="R10" s="62">
+        <v>6</v>
+      </c>
+      <c r="S10" s="62">
+        <v>3</v>
+      </c>
       <c r="T10" s="62"/>
       <c r="U10" s="62"/>
       <c r="V10" s="61">
         <f>IF(O10&gt;O11,1,0)+IF(P10&gt;P11,1,0)+IF(Q10&gt;Q11,1,0)+IF(R10&gt;R11,1,0)+IF(S10&gt;S11,1,0)+IF(T10&gt;T11,1,0)+IF(U10&gt;U11,1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W10" s="15"/>
       <c r="Y10" s="67"/>
@@ -8297,16 +8404,26 @@
       <c r="N11" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="62"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
+      <c r="O11" s="62">
+        <v>1</v>
+      </c>
+      <c r="P11" s="62">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="62">
+        <v>8</v>
+      </c>
+      <c r="R11" s="62">
+        <v>1</v>
+      </c>
+      <c r="S11" s="62">
+        <v>2</v>
+      </c>
       <c r="T11" s="62"/>
       <c r="U11" s="62"/>
       <c r="V11" s="61">
         <f>IF(O11&gt;O10,1,0)+IF(P11&gt;P10,1,0)+IF(Q11&gt;Q10,1,0)+IF(R11&gt;R10,1,0)+IF(S11&gt;S10,1,0)+IF(T11&gt;T10,1,0)+IF(U11&gt;U10,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11" s="67"/>
       <c r="Z11" s="67"/>
@@ -8707,21 +8824,35 @@
       <c r="K20" s="15"/>
       <c r="L20" s="12"/>
       <c r="M20" s="60" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="N20" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="O20" s="62"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="62"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="62"/>
-      <c r="T20" s="62"/>
-      <c r="U20" s="62"/>
+        <v>59</v>
+      </c>
+      <c r="O20" s="62">
+        <v>5</v>
+      </c>
+      <c r="P20" s="62">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="62">
+        <v>7</v>
+      </c>
+      <c r="R20" s="62">
+        <v>3</v>
+      </c>
+      <c r="S20" s="62">
+        <v>2</v>
+      </c>
+      <c r="T20" s="62">
+        <v>6</v>
+      </c>
+      <c r="U20" s="62">
+        <v>1</v>
+      </c>
       <c r="V20" s="61">
         <f>IF(O20&gt;O21,1,0)+IF(P20&gt;P21,1,0)+IF(Q20&gt;Q21,1,0)+IF(R20&gt;R21,1,0)+IF(S20&gt;S21,1,0)+IF(T20&gt;T21,1,0)+IF(U20&gt;U21,1,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W20" s="12"/>
       <c r="Y20" s="67"/>
@@ -8767,21 +8898,35 @@
       </c>
       <c r="K21" s="45"/>
       <c r="M21" s="60" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="N21" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="O21" s="62"/>
-      <c r="P21" s="62"/>
-      <c r="Q21" s="62"/>
-      <c r="R21" s="62"/>
-      <c r="S21" s="62"/>
-      <c r="T21" s="62"/>
-      <c r="U21" s="62"/>
+        <v>51</v>
+      </c>
+      <c r="O21" s="62">
+        <v>4</v>
+      </c>
+      <c r="P21" s="62">
+        <v>4</v>
+      </c>
+      <c r="Q21" s="62">
+        <v>2</v>
+      </c>
+      <c r="R21" s="62">
+        <v>6</v>
+      </c>
+      <c r="S21" s="62">
+        <v>5</v>
+      </c>
+      <c r="T21" s="62">
+        <v>3</v>
+      </c>
+      <c r="U21" s="62">
+        <v>2</v>
+      </c>
       <c r="V21" s="61">
         <f>IF(O21&gt;O20,1,0)+IF(P21&gt;P20,1,0)+IF(Q21&gt;Q20,1,0)+IF(R21&gt;R20,1,0)+IF(S21&gt;S20,1,0)+IF(T21&gt;T20,1,0)+IF(U21&gt;U20,1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W21" s="13"/>
       <c r="Y21" s="67"/>
@@ -8818,9 +8963,11 @@
       <c r="W22" s="13"/>
       <c r="X22" s="12"/>
       <c r="Y22" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z22" s="64"/>
+        <v>37</v>
+      </c>
+      <c r="Z22" s="64" t="s">
+        <v>51</v>
+      </c>
       <c r="AA22" s="62"/>
       <c r="AB22" s="62"/>
       <c r="AC22" s="62"/>
@@ -8857,9 +9004,11 @@
       <c r="V23" s="2"/>
       <c r="W23" s="13"/>
       <c r="Y23" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z23" s="64"/>
+        <v>33</v>
+      </c>
+      <c r="Z23" s="64" t="s">
+        <v>44</v>
+      </c>
       <c r="AA23" s="62"/>
       <c r="AB23" s="62"/>
       <c r="AC23" s="62"/>
@@ -8908,16 +9057,28 @@
       <c r="N24" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="O24" s="62"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
+      <c r="O24" s="62">
+        <v>6</v>
+      </c>
+      <c r="P24" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="63">
+        <v>5</v>
+      </c>
+      <c r="R24" s="63">
+        <v>1</v>
+      </c>
+      <c r="S24" s="63">
+        <v>4</v>
+      </c>
+      <c r="T24" s="63">
+        <v>5</v>
+      </c>
       <c r="U24" s="62"/>
       <c r="V24" s="61">
         <f>IF(O24&gt;O25,1,0)+IF(P24&gt;P25,1,0)+IF(Q24&gt;Q25,1,0)+IF(R24&gt;R25,1,0)+IF(S24&gt;S25,1,0)+IF(T24&gt;T25,1,0)+IF(U24&gt;U25,1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W24" s="15"/>
       <c r="Y24" s="67"/>
@@ -8965,16 +9126,28 @@
       <c r="N25" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="O25" s="62"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="63"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="63"/>
+      <c r="O25" s="62">
+        <v>4</v>
+      </c>
+      <c r="P25" s="63">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="63">
+        <v>1</v>
+      </c>
+      <c r="R25" s="63">
+        <v>4</v>
+      </c>
+      <c r="S25" s="63">
+        <v>3</v>
+      </c>
+      <c r="T25" s="63">
+        <v>2</v>
+      </c>
       <c r="U25" s="62"/>
       <c r="V25" s="61">
         <f>IF(O25&gt;O24,1,0)+IF(P25&gt;P24,1,0)+IF(Q25&gt;Q24,1,0)+IF(R25&gt;R24,1,0)+IF(S25&gt;S24,1,0)+IF(T25&gt;T24,1,0)+IF(U25&gt;U24,1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y25" s="67"/>
       <c r="Z25" s="67"/>

</xml_diff>